<commit_message>
[added]: few graphs added
</commit_message>
<xml_diff>
--- a/CURRENT WORK/SALT WORK - CODES/N = 3/LiCl - Done/Test Excelsheet for LiCl n=3.xlsx
+++ b/CURRENT WORK/SALT WORK - CODES/N = 3/LiCl - Done/Test Excelsheet for LiCl n=3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhanu\OneDrive\Desktop\Final-Year-Project\CURRENT WORK\SALT WORK - CODES\N = 3\LiCl - Done\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jda365-my.sharepoint.com/personal/dhanush_tamilselvan_jda_com/Documents/Desktop/Final-Year-Project/CURRENT WORK/SALT WORK - CODES/N = 3/LiCl - Done/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0A5512-7EC4-4A13-B82F-A9B402AFA8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E88A55E1-2FE1-4A75-8B73-96F5B642C0CF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="3" xr2:uid="{E88A55E1-2FE1-4A75-8B73-96F5B642C0CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet for finding Unknown LiCl" sheetId="1" r:id="rId1"/>
@@ -18815,43 +18815,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36D6104B-C9E0-42E8-AA2A-689EB615114A}">
   <dimension ref="A1:AV60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP27" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="AP30" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="BG33" sqref="BG33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="12.33203125" style="3" customWidth="1"/>
+    <col min="1" max="2" width="12.36328125" style="3" customWidth="1"/>
     <col min="3" max="3" width="12" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="3" customWidth="1"/>
-    <col min="5" max="6" width="13.109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" customWidth="1"/>
-    <col min="8" max="8" width="11.21875" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="6"/>
-    <col min="11" max="12" width="8.88671875" style="3"/>
-    <col min="13" max="13" width="7.109375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="3"/>
-    <col min="15" max="15" width="11.88671875" style="3" customWidth="1"/>
-    <col min="16" max="16" width="13.44140625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="12.44140625" style="3" customWidth="1"/>
-    <col min="18" max="18" width="15.5546875" style="3" customWidth="1"/>
-    <col min="19" max="19" width="8.88671875" style="6"/>
-    <col min="20" max="20" width="9.109375" customWidth="1"/>
-    <col min="22" max="22" width="14.21875" customWidth="1"/>
-    <col min="23" max="23" width="8.88671875" style="6"/>
-    <col min="26" max="26" width="8.88671875" style="6"/>
+    <col min="4" max="4" width="9.08984375" style="3" customWidth="1"/>
+    <col min="5" max="6" width="13.08984375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="11.36328125" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" customWidth="1"/>
+    <col min="9" max="9" width="8.90625" style="6"/>
+    <col min="11" max="12" width="8.90625" style="3"/>
+    <col min="13" max="13" width="7.08984375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="8.90625" style="3"/>
+    <col min="15" max="15" width="11.90625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="13.453125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="12.453125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="15.54296875" style="3" customWidth="1"/>
+    <col min="19" max="19" width="8.90625" style="6"/>
+    <col min="20" max="20" width="9.08984375" customWidth="1"/>
+    <col min="22" max="22" width="14.1796875" customWidth="1"/>
+    <col min="23" max="23" width="8.90625" style="6"/>
+    <col min="26" max="26" width="8.90625" style="6"/>
     <col min="29" max="29" width="12" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="12" style="6" customWidth="1"/>
     <col min="32" max="33" width="12" customWidth="1"/>
     <col min="34" max="34" width="12" style="8" customWidth="1"/>
     <col min="36" max="36" width="12" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.21875" customWidth="1"/>
-    <col min="39" max="39" width="8.88671875" style="6"/>
-    <col min="41" max="43" width="21.5546875" style="3" customWidth="1"/>
-    <col min="45" max="45" width="13.44140625" style="3" customWidth="1"/>
+    <col min="38" max="38" width="13.1796875" customWidth="1"/>
+    <col min="39" max="39" width="8.90625" style="6"/>
+    <col min="41" max="43" width="21.54296875" style="3" customWidth="1"/>
+    <col min="45" max="45" width="13.453125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:45" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C1" s="13" t="s">
         <v>26</v>
       </c>
@@ -18870,7 +18870,7 @@
       <c r="AH1"/>
       <c r="AM1"/>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.35">
       <c r="I2"/>
       <c r="L2" s="4" t="s">
         <v>1</v>
@@ -18893,7 +18893,7 @@
       <c r="AH2" s="3"/>
       <c r="AM2"/>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.35">
       <c r="I3"/>
       <c r="L3" s="4" t="s">
         <v>2</v>
@@ -18916,7 +18916,7 @@
       <c r="AH3" s="3"/>
       <c r="AM3"/>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.35">
       <c r="I4"/>
       <c r="S4"/>
       <c r="W4"/>
@@ -18933,7 +18933,7 @@
       <c r="AH4" s="3"/>
       <c r="AM4"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.35">
       <c r="I5"/>
       <c r="S5"/>
       <c r="W5"/>
@@ -18943,7 +18943,7 @@
       <c r="AM5"/>
       <c r="AO5" s="5"/>
     </row>
-    <row r="6" spans="1:45" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:45" ht="42" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -19019,7 +19019,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>1.0207999999999999</v>
       </c>
@@ -19159,7 +19159,7 @@
         <v>1.0198</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>1.0208999999999999</v>
       </c>
@@ -19295,7 +19295,7 @@
         <v>1.0125</v>
       </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>1.0212000000000001</v>
       </c>
@@ -19437,7 +19437,7 @@
         <v>1.0108999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>1.0215000000000001</v>
       </c>
@@ -19579,7 +19579,7 @@
         <v>0.99209999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>1.0218</v>
       </c>
@@ -19721,7 +19721,7 @@
         <v>0.98750000000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>1.0226999999999999</v>
       </c>
@@ -19863,7 +19863,7 @@
         <v>0.98640000000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>1.0238</v>
       </c>
@@ -20005,7 +20005,7 @@
         <v>0.97399999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>2.1970000000000001</v>
       </c>
@@ -20147,7 +20147,7 @@
         <v>1.1685000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>2.1970000000000001</v>
       </c>
@@ -20289,7 +20289,7 @@
         <v>1.1579999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>2.198</v>
       </c>
@@ -20431,7 +20431,7 @@
         <v>1.1493</v>
       </c>
     </row>
-    <row r="17" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>2.198</v>
       </c>
@@ -20573,7 +20573,7 @@
         <v>1.1323000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>2.1989999999999998</v>
       </c>
@@ -20715,7 +20715,7 @@
         <v>1.1226</v>
       </c>
     </row>
-    <row r="19" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>2.2010000000000001</v>
       </c>
@@ -20857,7 +20857,7 @@
         <v>1.1117999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>2.202</v>
       </c>
@@ -20999,7 +20999,7 @@
         <v>1.0942000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>3.94</v>
       </c>
@@ -21135,7 +21135,7 @@
         <v>1.4350000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>3.94</v>
       </c>
@@ -21271,7 +21271,7 @@
         <v>1.4131</v>
       </c>
     </row>
-    <row r="23" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>3.9420000000000002</v>
       </c>
@@ -21407,7 +21407,7 @@
         <v>1.3695999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>3.944</v>
       </c>
@@ -21543,7 +21543,7 @@
         <v>1.3434999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>3.9460000000000002</v>
       </c>
@@ -21679,7 +21679,7 @@
         <v>1.3196000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>3.95</v>
       </c>
@@ -21815,7 +21815,7 @@
         <v>1.3148</v>
       </c>
     </row>
-    <row r="27" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>6.3689999999999998</v>
       </c>
@@ -21951,7 +21951,7 @@
         <v>1.8464</v>
       </c>
     </row>
-    <row r="28" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>6.37</v>
       </c>
@@ -22087,7 +22087,7 @@
         <v>1.8107</v>
       </c>
     </row>
-    <row r="29" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>6.3710000000000004</v>
       </c>
@@ -22223,7 +22223,7 @@
         <v>1.7683</v>
       </c>
     </row>
-    <row r="30" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>6.3719999999999999</v>
       </c>
@@ -22359,7 +22359,7 @@
         <v>1.7264999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>6.375</v>
       </c>
@@ -22498,7 +22498,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>6.3789999999999996</v>
       </c>
@@ -22640,7 +22640,7 @@
         <v>1.8464</v>
       </c>
     </row>
-    <row r="33" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>6.3840000000000003</v>
       </c>
@@ -22782,7 +22782,7 @@
         <v>1.8107</v>
       </c>
     </row>
-    <row r="34" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>7.407</v>
       </c>
@@ -22924,7 +22924,7 @@
         <v>1.7683</v>
       </c>
     </row>
-    <row r="35" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>7.4080000000000004</v>
       </c>
@@ -23066,7 +23066,7 @@
         <v>1.7264999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>7.4089999999999998</v>
       </c>
@@ -23208,7 +23208,7 @@
         <v>1.6847000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>7.4109999999999996</v>
       </c>
@@ -23350,7 +23350,7 @@
         <v>1.6448</v>
       </c>
     </row>
-    <row r="38" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>7.4139999999999997</v>
       </c>
@@ -23492,7 +23492,7 @@
         <v>1.6043000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>7.4180000000000001</v>
       </c>
@@ -23634,7 +23634,7 @@
         <v>2.0259</v>
       </c>
     </row>
-    <row r="40" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>7.4240000000000004</v>
       </c>
@@ -23776,7 +23776,7 @@
         <v>1.9772000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>8.4920000000000009</v>
       </c>
@@ -23918,7 +23918,7 @@
         <v>1.9248000000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>8.4930000000000003</v>
       </c>
@@ -24060,7 +24060,7 @@
         <v>1.8772</v>
       </c>
     </row>
-    <row r="43" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>8.4939999999999998</v>
       </c>
@@ -24202,7 +24202,7 @@
         <v>1.8274999999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>8.4949999999999992</v>
       </c>
@@ -24344,7 +24344,7 @@
         <v>1.7834000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>8.4979999999999993</v>
       </c>
@@ -24486,7 +24486,7 @@
         <v>1.7375</v>
       </c>
     </row>
-    <row r="46" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>8.5020000000000007</v>
       </c>
@@ -24628,7 +24628,7 @@
         <v>2.2159</v>
       </c>
     </row>
-    <row r="47" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>8.5079999999999991</v>
       </c>
@@ -24770,7 +24770,7 @@
         <v>2.1575000000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>11.536</v>
       </c>
@@ -24912,7 +24912,7 @@
         <v>2.0958000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>11.537000000000001</v>
       </c>
@@ -25054,7 +25054,7 @@
         <v>2.0392000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>11.542</v>
       </c>
@@ -25196,7 +25196,7 @@
         <v>1.9770000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>11.545999999999999</v>
       </c>
@@ -25338,7 +25338,7 @@
         <v>1.9206000000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>11.532999999999999</v>
       </c>
@@ -25480,7 +25480,7 @@
         <v>1.8681000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>11.561999999999999</v>
       </c>
@@ -25622,7 +25622,7 @@
         <v>3.0539999999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>18.542000000000002</v>
       </c>
@@ -25764,7 +25764,7 @@
         <v>2.911</v>
       </c>
     </row>
-    <row r="55" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>18.544</v>
       </c>
@@ -25906,7 +25906,7 @@
         <v>2.7839999999999998</v>
       </c>
     </row>
-    <row r="56" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>18.547999999999998</v>
       </c>
@@ -26048,7 +26048,7 @@
         <v>2.6589999999999998</v>
       </c>
     </row>
-    <row r="57" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>18.550999999999998</v>
       </c>
@@ -26190,7 +26190,7 @@
         <v>2.5419999999999998</v>
       </c>
     </row>
-    <row r="58" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>18.559000000000001</v>
       </c>
@@ -26332,7 +26332,7 @@
         <v>2.4300000000000002</v>
       </c>
     </row>
-    <row r="59" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>18.57</v>
       </c>
@@ -26474,7 +26474,7 @@
         <v>2.3239999999999998</v>
       </c>
     </row>
-    <row r="60" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>18.585000000000001</v>
       </c>
@@ -26625,9 +26625,9 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>4.0775874274387613E-2</v>
       </c>
@@ -26635,7 +26635,7 @@
         <v>269.64318511963302</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>7.8356686165147529E-2</v>
       </c>
@@ -26643,7 +26643,7 @@
         <v>262.00130236596402</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0.10636557891682254</v>
       </c>
@@ -26651,7 +26651,7 @@
         <v>256.53937987343602</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>0.12627995151014915</v>
       </c>
@@ -26659,7 +26659,7 @@
         <v>252.17144479136999</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0.13907032302335606</v>
       </c>
@@ -26667,7 +26667,7 @@
         <v>247.81152426908801</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>0.16652314051620201</v>
       </c>
@@ -26675,7 +26675,7 @@
         <v>234.74378454191699</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>0.17817026128727032</v>
       </c>
@@ -26683,7 +26683,7 @@
         <v>230.38386401963501</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0.18387259980244294</v>
       </c>
@@ -26691,7 +26691,7 @@
         <v>226.03195805713699</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>0.19504312905448751</v>
       </c>
@@ -26699,7 +26699,7 @@
         <v>217.32814613214001</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0.20591199981246619</v>
       </c>
@@ -26707,7 +26707,7 @@
         <v>212.968225609857</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0.21123710620066591</v>
       </c>
@@ -26715,7 +26715,7 @@
         <v>206.44437394600101</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0.22932544647935366</v>
       </c>
@@ -26723,7 +26723,7 @@
         <v>196.64256733065</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0.24900791451437684</v>
       </c>
@@ -26731,7 +26731,7 @@
         <v>202.040373344909</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0.26998254423205381</v>
       </c>
@@ -26739,7 +26739,7 @@
         <v>209.60611778063401</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>0.2654233980266707</v>
       </c>
@@ -26747,7 +26747,7 @@
         <v>215.04399659381201</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0.27224096074934984</v>
       </c>
@@ -26755,7 +26755,7 @@
         <v>221.547811858209</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>0.27671613109853682</v>
       </c>
@@ -26763,7 +26763,7 @@
         <v>224.797715850461</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>0.28550336419818068</v>
       </c>
@@ -26771,7 +26771,7 @@
         <v>231.297523834966</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>0.2961916436392345</v>
       </c>
@@ -26779,7 +26779,7 @@
         <v>235.621378838222</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>0.30860291866516903</v>
       </c>
@@ -26787,7 +26787,7 @@
         <v>242.113172262944</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>0.31663674325714491</v>
       </c>
@@ -26795,7 +26795,7 @@
         <v>246.441034546092</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>0.33215700964059619</v>
       </c>
@@ -26803,7 +26803,7 @@
         <v>248.58092200831501</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>0.34334231492430106</v>
       </c>
@@ -26811,7 +26811,7 @@
         <v>258.33063398507198</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>0.35059333243870128</v>
       </c>
@@ -26819,7 +26819,7 @@
         <v>262.65849626822001</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>0.35768596294961891</v>
       </c>
@@ -26827,7 +26827,7 @@
         <v>265.90038570068901</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>0.36117449601146467</v>
       </c>
@@ -26835,7 +26835,7 @@
         <v>270.23626254362</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>0.36633681887053621</v>
       </c>
@@ -26843,7 +26843,7 @@
         <v>272.39618640530199</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>0.3697322641263695</v>
       </c>
@@ -26851,7 +26851,7 @@
         <v>275.64609039755499</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>0.37475774746673002</v>
       </c>
@@ -26859,7 +26859,7 @@
         <v>277.80601425923697</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>0.38457206184255815</v>
       </c>
@@ -26867,7 +26867,7 @@
         <v>279.95391628124401</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>0.39408303074749085</v>
       </c>
@@ -26875,7 +26875,7 @@
         <v>288.61765540732301</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>0.40178713334628252</v>
       </c>
@@ -26883,7 +26883,7 @@
         <v>292.94151041057899</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>0.41077733906176578</v>
       </c>
@@ -26891,7 +26891,7 @@
         <v>292.91746673122799</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>0.41662217782905875</v>
       </c>
@@ -26899,7 +26899,7 @@
         <v>300.50324756641203</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>0.42093027231234614</v>
       </c>
@@ -26907,7 +26907,7 @@
         <v>304.83511712945102</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>0.42797075263006773</v>
       </c>
@@ -26915,7 +26915,7 @@
         <v>310.24494498338601</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>0.43754462284357415</v>
       </c>
@@ -26923,7 +26923,7 @@
         <v>316.73273112821602</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>0.44549933705455752</v>
       </c>
@@ -26931,7 +26931,7 @@
         <v>323.224524552937</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>0.44939290996862896</v>
       </c>
@@ -26939,7 +26939,7 @@
         <v>330.81431266801297</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>0.45701828906663239</v>
       </c>
@@ -26947,7 +26947,7 @@
         <v>337.30610609273498</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>0.46565186528906</v>
       </c>
@@ -26955,7 +26955,7 @@
         <v>342.70791938688598</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>0.47518862224425584</v>
       </c>
@@ -26963,7 +26963,7 @@
         <v>345.93377969978701</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>0.4843909344130039</v>
       </c>
@@ -26971,7 +26971,7 @@
         <v>351.33158571404698</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>0.49327609160670688</v>
       </c>
@@ -26979,7 +26979,7 @@
         <v>354.55744602694801</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>0.50707914380920449</v>
       </c>
@@ -26987,7 +26987,7 @@
         <v>362.10716134310599</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>0.5101583399609565</v>
       </c>
@@ -26995,7 +26995,7 @@
         <v>365.35305805546699</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>0.51719567293302693</v>
       </c>
@@ -27003,7 +27003,7 @@
         <v>365.325007096224</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>0.53068066889261378</v>
       </c>
@@ -27011,7 +27011,7 @@
         <v>366.354878028418</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>0.52015015227707284</v>
       </c>
@@ -27019,7 +27019,7 @@
         <v>371.82882236062102</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>0.52112695966864042</v>
       </c>
@@ -27027,7 +27027,7 @@
         <v>379.42662503548098</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>0.52403366539742313</v>
       </c>
@@ -27035,7 +27035,7 @@
         <v>388.102386001235</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>0.52785482319818222</v>
       </c>
@@ -27043,7 +27043,7 @@
         <v>392.43024828438303</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>0.52880054526992226</v>
       </c>
@@ -27065,9 +27065,9 @@
       <selection activeCell="V6" sqref="V6:W37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -27075,7 +27075,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>4.0775874274387613E-2</v>
       </c>
@@ -27086,7 +27086,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>7.8356686165147529E-2</v>
       </c>
@@ -27094,7 +27094,7 @@
         <v>262.00130236596402</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>0.10636557891682254</v>
       </c>
@@ -27123,7 +27123,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0.12627995151014915</v>
       </c>
@@ -27131,7 +27131,7 @@
         <v>252.17144479136999</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>0.13907032302335606</v>
       </c>
@@ -27181,7 +27181,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>0.16652314051620201</v>
       </c>
@@ -27231,7 +27231,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0.17817026128727032</v>
       </c>
@@ -27281,7 +27281,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>0.18387259980244294</v>
       </c>
@@ -27331,7 +27331,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0.19504312905448751</v>
       </c>
@@ -27381,7 +27381,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0.20591199981246619</v>
       </c>
@@ -27431,7 +27431,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0.21123710620066591</v>
       </c>
@@ -27481,7 +27481,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0.22932544647935366</v>
       </c>
@@ -27531,7 +27531,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0.24900791451437684</v>
       </c>
@@ -27581,7 +27581,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>0.26998254423205381</v>
       </c>
@@ -27631,7 +27631,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0.2654233980266707</v>
       </c>
@@ -27681,7 +27681,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>0.27224096074934984</v>
       </c>
@@ -27731,7 +27731,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>0.27671613109853682</v>
       </c>
@@ -27781,7 +27781,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>0.28550336419818068</v>
       </c>
@@ -27831,7 +27831,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>0.2961916436392345</v>
       </c>
@@ -27881,7 +27881,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>0.30860291866516903</v>
       </c>
@@ -27931,7 +27931,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>0.31663674325714491</v>
       </c>
@@ -27981,7 +27981,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>0.33215700964059619</v>
       </c>
@@ -28031,7 +28031,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>0.34334231492430106</v>
       </c>
@@ -28081,7 +28081,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>0.35059333243870128</v>
       </c>
@@ -28131,7 +28131,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>0.35768596294961891</v>
       </c>
@@ -28175,7 +28175,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>0.36117449601146467</v>
       </c>
@@ -28219,7 +28219,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>0.36633681887053621</v>
       </c>
@@ -28263,7 +28263,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>0.3697322641263695</v>
       </c>
@@ -28301,7 +28301,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>0.37475774746673002</v>
       </c>
@@ -28339,7 +28339,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>0.38457206184255815</v>
       </c>
@@ -28377,7 +28377,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>0.39408303074749085</v>
       </c>
@@ -28415,7 +28415,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>0.40178713334628252</v>
       </c>
@@ -28453,7 +28453,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>0.41077733906176578</v>
       </c>
@@ -28485,7 +28485,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>0.41662217782905875</v>
       </c>
@@ -28517,7 +28517,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>0.42093027231234614</v>
       </c>
@@ -28549,7 +28549,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>0.42797075263006773</v>
       </c>
@@ -28581,7 +28581,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>0.43754462284357415</v>
       </c>
@@ -28607,7 +28607,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>0.44549933705455752</v>
       </c>
@@ -28633,7 +28633,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>0.44939290996862896</v>
       </c>
@@ -28659,7 +28659,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>0.45701828906663239</v>
       </c>
@@ -28685,7 +28685,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>0.46565186528906</v>
       </c>
@@ -28711,7 +28711,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>0.47518862224425584</v>
       </c>
@@ -28731,7 +28731,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>0.4843909344130039</v>
       </c>
@@ -28751,7 +28751,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>0.49327609160670688</v>
       </c>
@@ -28771,7 +28771,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>0.50707914380920449</v>
       </c>
@@ -28791,7 +28791,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>0.5101583399609565</v>
       </c>
@@ -28811,7 +28811,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>0.51719567293302693</v>
       </c>
@@ -28831,7 +28831,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>0.53068066889261378</v>
       </c>
@@ -28851,7 +28851,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>0.52015015227707284</v>
       </c>
@@ -28871,7 +28871,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>0.52112695966864042</v>
       </c>
@@ -28891,7 +28891,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>0.52403366539742313</v>
       </c>
@@ -28911,7 +28911,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>0.52785482319818222</v>
       </c>
@@ -28931,7 +28931,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>0.52880054526992226</v>
       </c>
@@ -28951,7 +28951,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D55">
         <v>1.6449999999999999E-2</v>
       </c>
@@ -28965,7 +28965,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D56">
         <v>1.1390000000000001E-2</v>
       </c>
@@ -28979,7 +28979,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D57">
         <v>5.2296299999999999E-3</v>
       </c>
@@ -28993,7 +28993,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G58">
         <v>0.34657900000000003</v>
       </c>
@@ -29001,7 +29001,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G59">
         <v>0.34863699999999997</v>
       </c>
@@ -29009,7 +29009,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G60">
         <v>0.35070299999999999</v>
       </c>
@@ -29017,7 +29017,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G61">
         <v>0.35277700000000001</v>
       </c>
@@ -29025,7 +29025,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G62">
         <v>0.35485899999999998</v>
       </c>
@@ -29033,7 +29033,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G63">
         <v>0.35694900000000002</v>
       </c>
@@ -29041,7 +29041,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G64">
         <v>0.35904599999999998</v>
       </c>
@@ -29049,7 +29049,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="65" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G65">
         <v>0.36115199999999997</v>
       </c>
@@ -29057,7 +29057,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="66" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G66">
         <v>0.35108099999999998</v>
       </c>
@@ -29065,7 +29065,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="67" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G67">
         <v>0.36538799999999999</v>
       </c>
@@ -29073,7 +29073,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="68" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G68">
         <v>0.36751800000000001</v>
       </c>
@@ -29081,7 +29081,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="69" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G69">
         <v>0.382415</v>
       </c>
@@ -29089,7 +29089,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="70" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G70">
         <v>0.37180200000000002</v>
       </c>
@@ -29097,7 +29097,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="71" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G71">
         <v>0.37611800000000001</v>
       </c>
@@ -29105,7 +29105,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="72" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G72">
         <v>0.37828800000000001</v>
       </c>
@@ -29113,7 +29113,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="73" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G73">
         <v>0.38308799999999998</v>
       </c>
@@ -29121,7 +29121,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="74" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G74">
         <v>0.38265199999999999</v>
       </c>
@@ -29129,7 +29129,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="75" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G75">
         <v>0.38484600000000002</v>
       </c>
@@ -29137,7 +29137,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="76" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G76">
         <v>0.387048</v>
       </c>
@@ -29145,7 +29145,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="77" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G77">
         <v>0.38925799999999999</v>
       </c>
@@ -29153,7 +29153,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="78" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G78">
         <v>0.37171599999999999</v>
       </c>
@@ -29161,7 +29161,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="79" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G79">
         <v>0.39370100000000002</v>
       </c>
@@ -29169,7 +29169,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="80" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G80">
         <v>0.39593499999999998</v>
       </c>
@@ -29177,7 +29177,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="81" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G81">
         <v>0.398177</v>
       </c>
@@ -29185,7 +29185,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="82" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G82">
         <v>0.40348800000000001</v>
       </c>
@@ -29193,7 +29193,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="83" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G83">
         <v>0.40268500000000002</v>
       </c>
@@ -29201,7 +29201,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="84" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G84">
         <v>0.40495100000000001</v>
       </c>
@@ -29209,7 +29209,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="85" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G85">
         <v>0.407225</v>
       </c>
@@ -29217,7 +29217,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="86" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G86">
         <v>0.40950700000000001</v>
       </c>
@@ -29225,7 +29225,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="87" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G87">
         <v>0.41179700000000002</v>
       </c>
@@ -29233,7 +29233,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="88" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G88">
         <v>0.41088400000000003</v>
       </c>
@@ -29241,7 +29241,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="89" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G89">
         <v>0.41640100000000002</v>
       </c>
@@ -29259,13 +29259,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{782205F6-3FFD-4338-A2A5-04E9D62A3720}">
   <dimension ref="A1:E210"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -29273,7 +29273,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -29287,7 +29287,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>4.0775874274387613E-2</v>
       </c>
@@ -29295,7 +29295,7 @@
         <v>269.64318511963302</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>7.8356686165147529E-2</v>
       </c>
@@ -29303,7 +29303,7 @@
         <v>262.00130236596402</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0.10636557891682254</v>
       </c>
@@ -29311,7 +29311,7 @@
         <v>256.53937987343602</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>0.12627995151014915</v>
       </c>
@@ -29319,7 +29319,7 @@
         <v>252.17144479136999</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>0.13907032302335606</v>
       </c>
@@ -29333,7 +29333,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0.16652314051620201</v>
       </c>
@@ -29347,7 +29347,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>0.17817026128727032</v>
       </c>
@@ -29361,7 +29361,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0.18387259980244294</v>
       </c>
@@ -29375,7 +29375,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0.19504312905448751</v>
       </c>
@@ -29389,7 +29389,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0.20591199981246619</v>
       </c>
@@ -29403,7 +29403,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0.21123710620066591</v>
       </c>
@@ -29417,7 +29417,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0.22932544647935366</v>
       </c>
@@ -29431,7 +29431,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>0.24900791451437684</v>
       </c>
@@ -29445,7 +29445,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0.26998254423205381</v>
       </c>
@@ -29459,7 +29459,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>0.2654233980266707</v>
       </c>
@@ -29473,7 +29473,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>0.27224096074934984</v>
       </c>
@@ -29487,7 +29487,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>0.27671613109853682</v>
       </c>
@@ -29501,7 +29501,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>0.28550336419818068</v>
       </c>
@@ -29515,7 +29515,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>0.2961916436392345</v>
       </c>
@@ -29529,7 +29529,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>0.30860291866516903</v>
       </c>
@@ -29543,7 +29543,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>0.31663674325714491</v>
       </c>
@@ -29557,7 +29557,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>0.33215700964059619</v>
       </c>
@@ -29571,7 +29571,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>0.34334231492430106</v>
       </c>
@@ -29585,7 +29585,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>0.35059333243870128</v>
       </c>
@@ -29599,7 +29599,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>0.35768596294961891</v>
       </c>
@@ -29613,7 +29613,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>0.36117449601146467</v>
       </c>
@@ -29627,7 +29627,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>0.36633681887053621</v>
       </c>
@@ -29641,7 +29641,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>0.3697322641263695</v>
       </c>
@@ -29655,7 +29655,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>0.37475774746673002</v>
       </c>
@@ -29669,7 +29669,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>0.38457206184255815</v>
       </c>
@@ -29683,7 +29683,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>0.39408303074749085</v>
       </c>
@@ -29697,7 +29697,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>0.40178713334628252</v>
       </c>
@@ -29711,7 +29711,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>0.41077733906176578</v>
       </c>
@@ -29725,7 +29725,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>0.41662217782905875</v>
       </c>
@@ -29739,7 +29739,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>0.42093027231234614</v>
       </c>
@@ -29753,7 +29753,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>0.42797075263006773</v>
       </c>
@@ -29767,7 +29767,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>0.43754462284357415</v>
       </c>
@@ -29781,7 +29781,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>0.44549933705455752</v>
       </c>
@@ -29795,7 +29795,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>0.44939290996862896</v>
       </c>
@@ -29809,7 +29809,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>0.45701828906663239</v>
       </c>
@@ -29823,7 +29823,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>0.46565186528906</v>
       </c>
@@ -29837,7 +29837,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>0.47518862224425584</v>
       </c>
@@ -29851,7 +29851,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>0.4843909344130039</v>
       </c>
@@ -29865,7 +29865,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>0.49327609160670688</v>
       </c>
@@ -29879,7 +29879,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>0.50707914380920449</v>
       </c>
@@ -29893,7 +29893,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>0.5101583399609565</v>
       </c>
@@ -29907,7 +29907,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>0.51719567293302693</v>
       </c>
@@ -29921,7 +29921,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>0.53068066889261378</v>
       </c>
@@ -29935,7 +29935,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>0.52015015227707284</v>
       </c>
@@ -29949,7 +29949,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>0.52112695966864042</v>
       </c>
@@ -29963,7 +29963,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>0.52403366539742313</v>
       </c>
@@ -29977,7 +29977,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>0.52785482319818222</v>
       </c>
@@ -29991,7 +29991,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>0.52880054526992226</v>
       </c>
@@ -30005,7 +30005,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D56">
         <v>0.18509999999999999</v>
       </c>
@@ -30013,7 +30013,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D57">
         <v>0.18598200000000001</v>
       </c>
@@ -30021,7 +30021,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D58">
         <v>0.187559</v>
       </c>
@@ -30029,7 +30029,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D59">
         <v>0.189142</v>
       </c>
@@ -30037,7 +30037,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D60">
         <v>0.19073100000000001</v>
       </c>
@@ -30045,7 +30045,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D61">
         <v>0.192326</v>
       </c>
@@ -30053,7 +30053,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D62">
         <v>0.19392699999999999</v>
       </c>
@@ -30061,7 +30061,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D63">
         <v>0.19553400000000001</v>
       </c>
@@ -30069,7 +30069,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D64">
         <v>0.19714699999999999</v>
       </c>
@@ -30077,7 +30077,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="65" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D65">
         <v>0.198765</v>
       </c>
@@ -30085,7 +30085,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="66" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D66">
         <v>0.20039000000000001</v>
       </c>
@@ -30093,7 +30093,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="67" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D67">
         <v>0.20202100000000001</v>
       </c>
@@ -30101,7 +30101,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="68" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D68">
         <v>0.20530100000000001</v>
       </c>
@@ -30109,7 +30109,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="69" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D69">
         <v>0.20695</v>
       </c>
@@ -30117,7 +30117,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="70" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D70">
         <v>0.20860500000000001</v>
       </c>
@@ -30125,7 +30125,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="71" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D71">
         <v>0.21026600000000001</v>
       </c>
@@ -30133,7 +30133,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="72" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D72">
         <v>0.21193300000000001</v>
       </c>
@@ -30141,7 +30141,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="73" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D73">
         <v>0.21360599999999999</v>
       </c>
@@ -30149,7 +30149,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="74" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D74">
         <v>0.215285</v>
       </c>
@@ -30157,7 +30157,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="75" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D75">
         <v>0.216969</v>
       </c>
@@ -30165,7 +30165,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="76" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D76">
         <v>0.21865999999999999</v>
       </c>
@@ -30173,7 +30173,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="77" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D77">
         <v>0.220357</v>
       </c>
@@ -30181,7 +30181,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="78" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D78">
         <v>0.22206000000000001</v>
       </c>
@@ -30189,7 +30189,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="79" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D79">
         <v>0.223769</v>
       </c>
@@ -30197,7 +30197,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="80" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D80">
         <v>0.22548399999999999</v>
       </c>
@@ -30205,7 +30205,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="81" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D81">
         <v>0.22720499999999999</v>
       </c>
@@ -30213,7 +30213,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="82" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D82">
         <v>0.228932</v>
       </c>
@@ -30221,7 +30221,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="83" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D83">
         <v>0.23066500000000001</v>
       </c>
@@ -30229,7 +30229,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="84" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D84">
         <v>0.232404</v>
       </c>
@@ -30237,7 +30237,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="85" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D85">
         <v>0.234149</v>
       </c>
@@ -30245,7 +30245,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="86" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D86">
         <v>0.24410200000000001</v>
       </c>
@@ -30253,7 +30253,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="87" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D87">
         <v>0.24571200000000001</v>
       </c>
@@ -30261,7 +30261,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="88" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D88">
         <v>0.24895600000000001</v>
       </c>
@@ -30269,7 +30269,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="89" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D89">
         <v>0.25058999999999998</v>
       </c>
@@ -30277,7 +30277,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="90" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D90">
         <v>0.25223200000000001</v>
       </c>
@@ -30285,7 +30285,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="91" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D91">
         <v>0.253882</v>
       </c>
@@ -30293,7 +30293,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="92" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D92">
         <v>0.25553999999999999</v>
       </c>
@@ -30301,7 +30301,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="93" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D93">
         <v>0.25827800000000001</v>
       </c>
@@ -30309,7 +30309,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="94" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D94">
         <v>0.25888</v>
       </c>
@@ -30317,7 +30317,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="95" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D95">
         <v>0.26056200000000002</v>
       </c>
@@ -30325,7 +30325,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="96" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D96">
         <v>0.26225199999999999</v>
       </c>
@@ -30333,7 +30333,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="97" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D97">
         <v>0.26235700000000001</v>
       </c>
@@ -30341,7 +30341,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="98" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D98">
         <v>0.26394899999999999</v>
       </c>
@@ -30349,7 +30349,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="99" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D99">
         <v>0.26565499999999997</v>
       </c>
@@ -30357,7 +30357,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="100" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D100">
         <v>0.26736900000000002</v>
       </c>
@@ -30365,7 +30365,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="101" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D101">
         <v>0.272559</v>
       </c>
@@ -30373,7 +30373,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="102" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D102">
         <v>0.276059</v>
       </c>
@@ -30381,7 +30381,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="103" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D103">
         <v>0.27629599999999999</v>
       </c>
@@ -30389,7 +30389,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="104" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D104">
         <v>0.27782099999999998</v>
       </c>
@@ -30397,7 +30397,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="105" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D105">
         <v>0.27959099999999998</v>
       </c>
@@ -30405,7 +30405,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="106" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D106">
         <v>0.28136899999999998</v>
       </c>
@@ -30413,7 +30413,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="107" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D107">
         <v>0.28315499999999999</v>
       </c>
@@ -30421,7 +30421,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="108" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D108">
         <v>0.28494900000000001</v>
       </c>
@@ -30429,7 +30429,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="109" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D109">
         <v>0.28675099999999998</v>
       </c>
@@ -30437,7 +30437,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="110" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D110">
         <v>0.28856100000000001</v>
       </c>
@@ -30445,7 +30445,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="111" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D111">
         <v>0.290379</v>
       </c>
@@ -30453,7 +30453,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="112" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D112">
         <v>0.29220499999999999</v>
       </c>
@@ -30461,7 +30461,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="113" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D113">
         <v>0.29403800000000002</v>
       </c>
@@ -30469,7 +30469,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="114" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D114">
         <v>0.29587999999999998</v>
       </c>
@@ -30477,7 +30477,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="115" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D115">
         <v>0.29772999999999999</v>
       </c>
@@ -30485,7 +30485,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="116" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D116">
         <v>0.29958800000000002</v>
       </c>
@@ -30493,7 +30493,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="117" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D117">
         <v>0.301454</v>
       </c>
@@ -30501,7 +30501,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="118" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D118">
         <v>0.30332799999999999</v>
       </c>
@@ -30509,7 +30509,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="119" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D119">
         <v>0.30709999999999998</v>
       </c>
@@ -30517,7 +30517,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="120" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D120">
         <v>0.30899799999999999</v>
       </c>
@@ -30525,7 +30525,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="121" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D121">
         <v>0.31281799999999998</v>
       </c>
@@ -30533,7 +30533,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="122" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D122">
         <v>0.31667000000000001</v>
       </c>
@@ -30541,7 +30541,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="123" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D123">
         <v>0.318608</v>
       </c>
@@ -30549,7 +30549,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="124" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D124">
         <v>0.32055400000000001</v>
       </c>
@@ -30557,7 +30557,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="125" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D125">
         <v>0.32446999999999998</v>
       </c>
@@ -30565,7 +30565,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="126" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D126">
         <v>0.330403</v>
       </c>
@@ -30573,7 +30573,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="127" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D127">
         <v>0.33417400000000003</v>
       </c>
@@ -30581,7 +30581,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="128" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D128">
         <v>0.334399</v>
       </c>
@@ -30589,7 +30589,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="129" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D129">
         <v>0.33842699999999998</v>
       </c>
@@ -30597,7 +30597,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="130" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D130">
         <v>0.34045300000000001</v>
       </c>
@@ -30605,7 +30605,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="131" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D131">
         <v>0.34338400000000002</v>
       </c>
@@ -30613,7 +30613,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="132" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D132">
         <v>0.34369699999999997</v>
       </c>
@@ -30621,7 +30621,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="133" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D133">
         <v>0.34657900000000003</v>
       </c>
@@ -30629,7 +30629,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="134" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D134">
         <v>0.34863699999999997</v>
       </c>
@@ -30637,7 +30637,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="135" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D135">
         <v>0.35070299999999999</v>
       </c>
@@ -30645,7 +30645,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="136" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D136">
         <v>0.35108099999999998</v>
       </c>
@@ -30653,7 +30653,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="137" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D137">
         <v>0.35277700000000001</v>
       </c>
@@ -30661,7 +30661,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="138" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D138">
         <v>0.35485899999999998</v>
       </c>
@@ -30669,7 +30669,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="139" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D139">
         <v>0.35694900000000002</v>
       </c>
@@ -30677,7 +30677,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="140" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D140">
         <v>0.35904599999999998</v>
       </c>
@@ -30685,7 +30685,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="141" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D141">
         <v>0.36115199999999997</v>
       </c>
@@ -30693,7 +30693,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="142" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D142">
         <v>0.36538799999999999</v>
       </c>
@@ -30701,7 +30701,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="143" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D143">
         <v>0.38484600000000002</v>
       </c>
@@ -30709,7 +30709,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="144" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D144">
         <v>0.387048</v>
       </c>
@@ -30717,7 +30717,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="145" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D145">
         <v>0.38925799999999999</v>
       </c>
@@ -30725,7 +30725,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="146" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D146">
         <v>0.39370100000000002</v>
       </c>
@@ -30733,7 +30733,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="147" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D147">
         <v>0.39593499999999998</v>
       </c>
@@ -30741,7 +30741,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="148" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D148">
         <v>0.398177</v>
       </c>
@@ -30749,7 +30749,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="149" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D149">
         <v>0.40268500000000002</v>
       </c>
@@ -30757,7 +30757,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="150" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D150">
         <v>0.40348800000000001</v>
       </c>
@@ -30765,7 +30765,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="151" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D151">
         <v>0.40495100000000001</v>
       </c>
@@ -30773,7 +30773,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="152" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D152">
         <v>0.407225</v>
       </c>
@@ -30781,7 +30781,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="153" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D153">
         <v>0.42696200000000001</v>
       </c>
@@ -30789,7 +30789,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="154" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D154">
         <v>0.42812600000000001</v>
       </c>
@@ -30797,7 +30797,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="155" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="155" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D155">
         <v>0.42928899999999998</v>
       </c>
@@ -30805,7 +30805,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="156" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D156">
         <v>0.43276599999999998</v>
       </c>
@@ -30813,7 +30813,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="157" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="157" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D157">
         <v>0.43392199999999997</v>
       </c>
@@ -30821,7 +30821,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="158" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="158" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D158">
         <v>0.43507499999999999</v>
       </c>
@@ -30829,7 +30829,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="159" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D159">
         <v>0.43737700000000002</v>
       </c>
@@ -30837,7 +30837,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="160" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="160" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D160">
         <v>0.43967200000000001</v>
       </c>
@@ -30845,7 +30845,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="161" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D161">
         <v>0.44081700000000001</v>
       </c>
@@ -30853,7 +30853,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="162" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D162">
         <v>0.44195899999999999</v>
       </c>
@@ -30861,7 +30861,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="163" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D163">
         <v>0.44416699999999998</v>
       </c>
@@ -30869,7 +30869,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="164" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D164">
         <v>0.44424000000000002</v>
       </c>
@@ -30877,7 +30877,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="165" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D165">
         <v>0.44764700000000002</v>
       </c>
@@ -30885,7 +30885,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="166" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D166">
         <v>0.449909</v>
       </c>
@@ -30893,7 +30893,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="167" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D167">
         <v>0.453289</v>
       </c>
@@ -30901,7 +30901,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="168" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D168">
         <v>0.45553500000000002</v>
       </c>
@@ -30909,7 +30909,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="169" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D169">
         <v>0.45665299999999998</v>
       </c>
@@ -30917,7 +30917,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="170" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D170">
         <v>0.45777000000000001</v>
       </c>
@@ -30925,7 +30925,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="171" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D171">
         <v>0.46111200000000002</v>
       </c>
@@ -30933,7 +30933,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="172" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D172">
         <v>0.46222299999999999</v>
       </c>
@@ -30941,7 +30941,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="173" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D173">
         <v>0.47289599999999998</v>
       </c>
@@ -30949,7 +30949,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="174" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D174">
         <v>0.47489100000000001</v>
       </c>
@@ -30957,7 +30957,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="175" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D175">
         <v>0.47689999999999999</v>
       </c>
@@ -30965,7 +30965,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="176" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D176">
         <v>0.47892299999999999</v>
       </c>
@@ -30973,7 +30973,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="177" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="177" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D177">
         <v>0.48065600000000003</v>
       </c>
@@ -30981,7 +30981,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="178" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="178" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D178">
         <v>0.48096</v>
       </c>
@@ -30989,7 +30989,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="179" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="179" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D179">
         <v>0.48301100000000002</v>
       </c>
@@ -30997,7 +30997,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="180" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="180" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D180">
         <v>0.48507499999999998</v>
       </c>
@@ -31005,7 +31005,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="181" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="181" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D181">
         <v>0.48715399999999998</v>
       </c>
@@ -31013,7 +31013,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="182" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="182" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D182">
         <v>0.493475</v>
       </c>
@@ -31021,7 +31021,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="183" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D183">
         <v>0.500143</v>
       </c>
@@ -31029,7 +31029,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="184" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D184">
         <v>0.50428899999999999</v>
       </c>
@@ -31037,7 +31037,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="185" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="185" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D185">
         <v>0.50871299999999997</v>
       </c>
@@ -31045,7 +31045,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="186" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="186" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D186">
         <v>0.51049100000000003</v>
       </c>
@@ -31053,7 +31053,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="187" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="187" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D187">
         <v>0.51319199999999998</v>
       </c>
@@ -31061,7 +31061,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="188" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="188" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D188">
         <v>0.51545300000000005</v>
       </c>
@@ -31069,7 +31069,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="189" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="189" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D189">
         <v>0.52001600000000003</v>
       </c>
@@ -31077,7 +31077,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="190" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="190" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D190">
         <v>0.52231899999999998</v>
       </c>
@@ -31085,7 +31085,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="191" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="191" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D191">
         <v>0.52851999999999999</v>
       </c>
@@ -31093,7 +31093,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="192" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="192" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D192">
         <v>0.53018699999999996</v>
       </c>
@@ -31101,7 +31101,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="193" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="193" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D193">
         <v>0.53074699999999997</v>
       </c>
@@ -31109,7 +31109,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="194" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="194" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D194">
         <v>0.53104200000000001</v>
       </c>
@@ -31117,7 +31117,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="195" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="195" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D195">
         <v>0.53166199999999997</v>
       </c>
@@ -31125,7 +31125,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="196" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="196" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D196">
         <v>0.53198699999999999</v>
       </c>
@@ -31133,7 +31133,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="197" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="197" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D197">
         <v>0.53232199999999996</v>
       </c>
@@ -31141,7 +31141,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="198" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="198" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D198">
         <v>0.53338600000000003</v>
       </c>
@@ -31149,7 +31149,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="199" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="199" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D199">
         <v>0.53414600000000001</v>
       </c>
@@ -31157,7 +31157,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="200" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="200" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D200">
         <v>0.53494600000000003</v>
       </c>
@@ -31165,7 +31165,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="201" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="201" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D201">
         <v>0.53536099999999998</v>
       </c>
@@ -31173,7 +31173,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="202" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="202" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D202">
         <v>0.53622099999999995</v>
       </c>
@@ -31181,7 +31181,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="203" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="203" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D203">
         <v>0.53712099999999996</v>
       </c>
@@ -31189,7 +31189,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="204" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="204" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D204">
         <v>0.53758600000000001</v>
       </c>
@@ -31197,7 +31197,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="205" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="205" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D205">
         <v>0.53805999999999998</v>
       </c>
@@ -31205,7 +31205,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="206" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="206" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D206">
         <v>0.53847500000000004</v>
       </c>
@@ -31213,7 +31213,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="207" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="207" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D207">
         <v>0.53903999999999996</v>
       </c>
@@ -31221,7 +31221,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="208" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="208" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D208">
         <v>0.54005999999999998</v>
       </c>
@@ -31229,7 +31229,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="209" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="209" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D209">
         <v>0.54221900000000001</v>
       </c>
@@ -31237,7 +31237,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="210" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="210" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D210">
         <v>0.54278400000000004</v>
       </c>
@@ -31263,15 +31263,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010054E8EBE579ED724DA6862405C7970F81" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="86c5e3b6225d101e522740491cefce85">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="49fa8af8-517d-491f-a3d5-7cf68fb985f9" xmlns:ns4="5d848a0f-dbe6-471c-a407-bb7a402dc859" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a6c024ab2e87b0647c7181ba4225cb0c" ns3:_="" ns4:_="">
     <xsd:import namespace="49fa8af8-517d-491f-a3d5-7cf68fb985f9"/>
@@ -31500,6 +31491,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AC3A44B-2E43-454A-BBA7-EBDF5C93942F}">
   <ds:schemaRefs>
@@ -31518,14 +31518,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C69340E-2751-479C-A826-08E03A5B21D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE99C8A8-65B8-4C1C-AC8C-1B7793729012}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -31542,4 +31534,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C69340E-2751-479C-A826-08E03A5B21D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[updated]: graph changes are implemented
</commit_message>
<xml_diff>
--- a/CURRENT WORK/SALT WORK - CODES/N = 3/LiCl - Done/Test Excelsheet for LiCl n=3.xlsx
+++ b/CURRENT WORK/SALT WORK - CODES/N = 3/LiCl - Done/Test Excelsheet for LiCl n=3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhanu\OneDrive\Desktop\Final-Year-Project\CURRENT WORK\SALT WORK - CODES\N = 3\LiCl - Done\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C7D565-147A-4223-9502-6EA1C180B9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93867D99-CC85-4827-9ADE-CAAC7A14BBDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E88A55E1-2FE1-4A75-8B73-96F5B642C0CF}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="3" xr2:uid="{E88A55E1-2FE1-4A75-8B73-96F5B642C0CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet for finding Unknown LiCl" sheetId="1" r:id="rId1"/>
@@ -199,7 +199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>n=3</t>
   </si>
@@ -325,6 +325,9 @@
   </si>
   <si>
     <t>For graph purpose</t>
+  </si>
+  <si>
+    <t>Till End</t>
   </si>
 </sst>
 </file>
@@ -2043,376 +2046,6 @@
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Experimental Data</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="7"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:srgbClr val="C00000"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Comparision graph'!$A$3:$A$55</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="53"/>
-                <c:pt idx="0">
-                  <c:v>4.0775874274387613E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.8356686165147529E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.10636557891682254</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.12627995151014915</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.13907032302335606</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.16652314051620201</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.17817026128727032</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.18387259980244294</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.19504312905448751</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.20591199981246619</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.21123710620066591</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.22932544647935366</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.24900791451437684</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.26998254423205381</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.2654233980266707</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.27224096074934984</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.27671613109853682</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.28550336419818068</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.2961916436392345</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.30860291866516903</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.31663674325714491</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.33215700964059619</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.34334231492430106</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.35059333243870128</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.35768596294961891</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.36117449601146467</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.36633681887053621</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.3697322641263695</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.37475774746673002</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.38457206184255815</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.39408303074749085</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.40178713334628252</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.41077733906176578</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.41662217782905875</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.42093027231234614</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.42797075263006773</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.43754462284357415</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.44549933705455752</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.44939290996862896</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.45701828906663239</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.46565186528906</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.47518862224425584</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.4843909344130039</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.49327609160670688</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.50707914380920449</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.5101583399609565</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.51719567293302693</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.53068066889261378</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.52015015227707284</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.52112695966864042</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.52403366539742313</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0.52785482319818222</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0.52880054526992226</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Comparision graph'!$B$3:$B$55</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="53"/>
-                <c:pt idx="0">
-                  <c:v>269.64318511963302</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>262.00130236596402</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256.53937987343602</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>252.17144479136999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>247.81152426908801</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>234.74378454191699</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>230.38386401963501</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>226.03195805713699</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>217.32814613214001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>212.968225609857</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>206.44437394600101</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>196.64256733065</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>202.040373344909</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>209.60611778063401</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>215.04399659381201</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>221.547811858209</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>224.797715850461</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>231.297523834966</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>235.621378838222</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>242.113172262944</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>246.441034546092</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>248.58092200831501</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>258.33063398507198</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>262.65849626822001</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>265.90038570068901</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>270.23626254362</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>272.39618640530199</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>275.64609039755499</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>277.80601425923697</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>279.95391628124401</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>288.61765540732301</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>292.94151041057899</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>292.91746673122799</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>300.50324756641203</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>304.83511712945102</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>310.24494498338601</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>316.73273112821602</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>323.224524552937</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>330.81431266801297</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>337.30610609273498</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>342.70791938688598</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>345.93377969978701</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>351.33158571404698</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>354.55744602694801</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>362.10716134310599</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>365.35305805546699</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>365.325007096224</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>366.354878028418</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>371.82882236062102</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>379.42662503548098</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>388.102386001235</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>392.43024828438303</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>396.77013240720601</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1D5E-4321-A92C-85C792284B8A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2423,6 +2056,394 @@
         </c:dLbls>
         <c:axId val="1709988112"/>
         <c:axId val="2111475280"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:v>Experimental Data</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="7"/>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:srgbClr val="C00000"/>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Comparision graph'!$A$3:$A$55</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="53"/>
+                      <c:pt idx="0">
+                        <c:v>4.0775874274387613E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>7.8356686165147529E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.10636557891682254</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.12627995151014915</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.13907032302335606</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.16652314051620201</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.17817026128727032</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.18387259980244294</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.19504312905448751</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.20591199981246619</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.21123710620066591</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.22932544647935366</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.24900791451437684</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.26998254423205381</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.2654233980266707</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0.27224096074934984</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0.27671613109853682</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>0.28550336419818068</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>0.2961916436392345</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>0.30860291866516903</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>0.31663674325714491</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>0.33215700964059619</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>0.34334231492430106</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>0.35059333243870128</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>0.35768596294961891</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>0.36117449601146467</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>0.36633681887053621</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>0.3697322641263695</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>0.37475774746673002</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>0.38457206184255815</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>0.39408303074749085</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>0.40178713334628252</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>0.41077733906176578</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>0.41662217782905875</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>0.42093027231234614</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>0.42797075263006773</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>0.43754462284357415</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>0.44549933705455752</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>0.44939290996862896</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>0.45701828906663239</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>0.46565186528906</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>0.47518862224425584</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>0.4843909344130039</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>0.49327609160670688</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>0.50707914380920449</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>0.5101583399609565</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>0.51719567293302693</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>0.53068066889261378</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>0.52015015227707284</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>0.52112695966864042</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>0.52403366539742313</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>0.52785482319818222</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>0.52880054526992226</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Comparision graph'!$B$3:$B$55</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="53"/>
+                      <c:pt idx="0">
+                        <c:v>269.64318511963302</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>262.00130236596402</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>256.53937987343602</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>252.17144479136999</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>247.81152426908801</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>234.74378454191699</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>230.38386401963501</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>226.03195805713699</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>217.32814613214001</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>212.968225609857</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>206.44437394600101</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>196.64256733065</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>202.040373344909</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>209.60611778063401</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>215.04399659381201</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>221.547811858209</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>224.797715850461</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>231.297523834966</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>235.621378838222</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>242.113172262944</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>246.441034546092</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>248.58092200831501</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>258.33063398507198</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>262.65849626822001</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>265.90038570068901</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>270.23626254362</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>272.39618640530199</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>275.64609039755499</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>277.80601425923697</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>279.95391628124401</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>288.61765540732301</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>292.94151041057899</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>292.91746673122799</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>300.50324756641203</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>304.83511712945102</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>310.24494498338601</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>316.73273112821602</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>323.224524552937</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>330.81431266801297</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>337.30610609273498</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>342.70791938688598</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>345.93377969978701</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>351.33158571404698</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>354.55744602694801</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>362.10716134310599</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>365.35305805546699</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>365.325007096224</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>366.354878028418</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>371.82882236062102</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>379.42662503548098</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>388.102386001235</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>392.43024828438303</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>396.77013240720601</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-1D5E-4321-A92C-85C792284B8A}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -2451,607 +2472,430 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="232"/>
+                <c:pt idx="0">
+                  <c:v>2.7025400000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2099999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6417199999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.2013399999999999E-2</c:v>
+                </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.7025400000000002E-2</c:v>
+                  <c:v>4.68511E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.2099999999999997E-2</c:v>
+                  <c:v>5.3877500000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.6417199999999997E-2</c:v>
+                  <c:v>5.86314E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.2013399999999999E-2</c:v>
+                  <c:v>6.9841600000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.68511E-2</c:v>
+                  <c:v>7.2817499999999993E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.3877500000000002E-2</c:v>
+                  <c:v>7.8476400000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.86314E-2</c:v>
+                  <c:v>8.2672899999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.9841600000000004E-2</c:v>
+                  <c:v>8.6788000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.2817499999999993E-2</c:v>
+                  <c:v>0.123644</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.8476400000000002E-2</c:v>
+                  <c:v>0.12687899999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8.2672899999999994E-2</c:v>
+                  <c:v>0.13003600000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8.6788000000000004E-2</c:v>
+                  <c:v>0.13311300000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.3631400000000004E-2</c:v>
+                  <c:v>0.13611100000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9.4769500000000007E-2</c:v>
+                  <c:v>0.13902900000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.8624500000000004E-2</c:v>
+                  <c:v>0.14186799999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.10026</c:v>
+                  <c:v>0.14462700000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.104265</c:v>
+                  <c:v>0.14730599999999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.11694400000000001</c:v>
+                  <c:v>0.14990500000000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.123644</c:v>
+                  <c:v>0.152425</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.12687899999999999</c:v>
+                  <c:v>0.154864</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.13003600000000001</c:v>
+                  <c:v>0.157223</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.13311300000000001</c:v>
+                  <c:v>0.15950300000000001</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.13611100000000001</c:v>
+                  <c:v>0.16170300000000001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.13902900000000001</c:v>
+                  <c:v>0.163822</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.14186799999999999</c:v>
+                  <c:v>0.16586200000000001</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.14462700000000001</c:v>
+                  <c:v>0.167822</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.14730599999999999</c:v>
+                  <c:v>0.16970099999999999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.14990500000000001</c:v>
+                  <c:v>0.17150099999999999</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.152425</c:v>
+                  <c:v>0.17322100000000001</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.154864</c:v>
+                  <c:v>0.17486099999999999</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.157223</c:v>
+                  <c:v>0.19392699999999999</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.15950300000000001</c:v>
+                  <c:v>0.19553400000000001</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.16170300000000001</c:v>
+                  <c:v>0.19714699999999999</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.163822</c:v>
+                  <c:v>0.198765</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.16586200000000001</c:v>
+                  <c:v>0.20039000000000001</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.167822</c:v>
+                  <c:v>0.20202100000000001</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.16970099999999999</c:v>
+                  <c:v>0.20530100000000001</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.17150099999999999</c:v>
+                  <c:v>0.20695</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.17322100000000001</c:v>
+                  <c:v>0.20860500000000001</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.17486099999999999</c:v>
+                  <c:v>0.21026600000000001</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.17642099999999999</c:v>
+                  <c:v>0.21193300000000001</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.1779</c:v>
+                  <c:v>0.21360599999999999</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.17929999999999999</c:v>
+                  <c:v>0.215285</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.18062</c:v>
+                  <c:v>0.216969</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.18185999999999999</c:v>
+                  <c:v>0.21865999999999999</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.18284700000000001</c:v>
+                  <c:v>0.220357</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.18301999999999999</c:v>
+                  <c:v>0.22206000000000001</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.18410000000000001</c:v>
+                  <c:v>0.223769</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.18441199999999999</c:v>
+                  <c:v>0.22548399999999999</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.189142</c:v>
+                  <c:v>0.22720499999999999</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.19073100000000001</c:v>
+                  <c:v>0.228932</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.192326</c:v>
+                  <c:v>0.23066500000000001</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.19392699999999999</c:v>
+                  <c:v>0.232404</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.19553400000000001</c:v>
+                  <c:v>0.234149</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.19714699999999999</c:v>
+                  <c:v>0.24410200000000001</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.198765</c:v>
+                  <c:v>0.24571200000000001</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.20039000000000001</c:v>
+                  <c:v>0.24895600000000001</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.20202100000000001</c:v>
+                  <c:v>0.25058999999999998</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.20530100000000001</c:v>
+                  <c:v>0.25223200000000001</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.20695</c:v>
+                  <c:v>0.253882</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.20860500000000001</c:v>
+                  <c:v>0.25553999999999999</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.21026600000000001</c:v>
+                  <c:v>0.25827800000000001</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.21193300000000001</c:v>
+                  <c:v>0.25888</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.21360599999999999</c:v>
+                  <c:v>0.27629599999999999</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.215285</c:v>
+                  <c:v>0.28675099999999998</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.216969</c:v>
+                  <c:v>0.28856100000000001</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.21865999999999999</c:v>
+                  <c:v>0.290379</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.220357</c:v>
+                  <c:v>0.29220499999999999</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.22206000000000001</c:v>
+                  <c:v>0.29403800000000002</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.223769</c:v>
+                  <c:v>0.29587999999999998</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.22548399999999999</c:v>
+                  <c:v>0.29772999999999999</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.22720499999999999</c:v>
+                  <c:v>0.29958800000000002</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.228932</c:v>
+                  <c:v>0.301454</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.23066500000000001</c:v>
+                  <c:v>0.30332799999999999</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.232404</c:v>
+                  <c:v>0.30709999999999998</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.234149</c:v>
+                  <c:v>0.30899799999999999</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.24410200000000001</c:v>
+                  <c:v>0.31281799999999998</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.24571200000000001</c:v>
+                  <c:v>0.31667000000000001</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.24895600000000001</c:v>
+                  <c:v>0.318608</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.25058999999999998</c:v>
+                  <c:v>0.32055400000000001</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.25223200000000001</c:v>
+                  <c:v>0.32446999999999998</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.253882</c:v>
+                  <c:v>0.330403</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.25553999999999999</c:v>
+                  <c:v>0.35904599999999998</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.25827800000000001</c:v>
+                  <c:v>0.36115199999999997</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.25888</c:v>
+                  <c:v>0.36538799999999999</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.26056200000000002</c:v>
+                  <c:v>0.38484600000000002</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.26225199999999999</c:v>
+                  <c:v>0.387048</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.26235700000000001</c:v>
+                  <c:v>0.38925799999999999</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.26394899999999999</c:v>
+                  <c:v>0.39370100000000002</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.26565499999999997</c:v>
+                  <c:v>0.39593499999999998</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.26736900000000002</c:v>
+                  <c:v>0.398177</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.272559</c:v>
+                  <c:v>0.40268500000000002</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.276059</c:v>
+                  <c:v>0.40495100000000001</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.27629599999999999</c:v>
+                  <c:v>0.407225</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.27782099999999998</c:v>
+                  <c:v>0.42696200000000001</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.27959099999999998</c:v>
+                  <c:v>0.42812600000000001</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.28136899999999998</c:v>
+                  <c:v>0.42928899999999998</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>0.28315499999999999</c:v>
+                  <c:v>0.43276599999999998</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>0.28494900000000001</c:v>
+                  <c:v>0.43392199999999997</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>0.28675099999999998</c:v>
+                  <c:v>0.43507499999999999</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>0.28856100000000001</c:v>
+                  <c:v>0.43737700000000002</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>0.290379</c:v>
+                  <c:v>0.449909</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>0.29220499999999999</c:v>
+                  <c:v>0.453289</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>0.29403800000000002</c:v>
+                  <c:v>0.45553500000000002</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>0.29587999999999998</c:v>
+                  <c:v>0.45665299999999998</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>0.29772999999999999</c:v>
+                  <c:v>0.45777000000000001</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>0.29958800000000002</c:v>
+                  <c:v>0.46111200000000002</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>0.301454</c:v>
+                  <c:v>0.46222299999999999</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>0.30332799999999999</c:v>
+                  <c:v>0.47289599999999998</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>0.30709999999999998</c:v>
+                  <c:v>0.47489100000000001</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>0.30899799999999999</c:v>
+                  <c:v>0.47689999999999999</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>0.31281799999999998</c:v>
+                  <c:v>0.47892299999999999</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>0.31667000000000001</c:v>
+                  <c:v>0.48715399999999998</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>0.318608</c:v>
+                  <c:v>0.51049100000000003</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>0.32055400000000001</c:v>
+                  <c:v>0.51319199999999998</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>0.32446999999999998</c:v>
+                  <c:v>0.51545300000000005</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>0.330403</c:v>
+                  <c:v>0.52001600000000003</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>0.33417400000000003</c:v>
+                  <c:v>0.52231899999999998</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>0.334399</c:v>
+                  <c:v>0.52851999999999999</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>0.33842699999999998</c:v>
+                  <c:v>0.53018699999999996</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>0.34045300000000001</c:v>
+                  <c:v>0.53074699999999997</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>0.34338400000000002</c:v>
+                  <c:v>0.53104200000000001</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>0.34369699999999997</c:v>
+                  <c:v>0.53166199999999997</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>0.34657900000000003</c:v>
+                  <c:v>0.53198699999999999</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>0.34863699999999997</c:v>
+                  <c:v>0.53232199999999996</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>0.35070299999999999</c:v>
+                  <c:v>0.53338600000000003</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>0.35108099999999998</c:v>
+                  <c:v>0.53414600000000001</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>0.35277700000000001</c:v>
+                  <c:v>0.53494600000000003</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>0.35485899999999998</c:v>
+                  <c:v>0.53536099999999998</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>0.35694900000000002</c:v>
+                  <c:v>0.53622099999999995</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>0.35904599999999998</c:v>
+                  <c:v>0.53712099999999996</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>0.36115199999999997</c:v>
+                  <c:v>0.53758600000000001</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>0.36538799999999999</c:v>
+                  <c:v>0.53805999999999998</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>0.38484600000000002</c:v>
+                  <c:v>0.53847500000000004</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>0.387048</c:v>
+                  <c:v>0.53903999999999996</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>0.38925799999999999</c:v>
+                  <c:v>0.54005999999999998</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>0.39370100000000002</c:v>
+                  <c:v>0.54221900000000001</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>0.39593499999999998</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>0.398177</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>0.40268500000000002</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>0.40348800000000001</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>0.40495100000000001</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>0.407225</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>0.42696200000000001</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>0.42812600000000001</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>0.42928899999999998</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>0.43276599999999998</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>0.43392199999999997</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>0.43507499999999999</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>0.43737700000000002</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>0.43967200000000001</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>0.44081700000000001</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>0.44195899999999999</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>0.44416699999999998</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>0.44424000000000002</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>0.44764700000000002</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>0.449909</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>0.453289</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>0.45553500000000002</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>0.45665299999999998</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>0.45777000000000001</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>0.46111200000000002</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>0.46222299999999999</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>0.47289599999999998</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>0.47489100000000001</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>0.47689999999999999</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>0.47892299999999999</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>0.48065600000000003</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>0.48096</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>0.48301100000000002</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>0.48507499999999998</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>0.48715399999999998</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>0.493475</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>0.500143</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>0.50428899999999999</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>0.50871299999999997</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>0.51049100000000003</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>0.51319199999999998</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>0.51545300000000005</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>0.52001600000000003</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>0.52231899999999998</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>0.52851999999999999</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>0.53018699999999996</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>0.53074699999999997</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>0.53104200000000001</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>0.53166199999999997</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>0.53198699999999999</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>0.53232199999999996</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>0.53338600000000003</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>0.53414600000000001</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>0.53494600000000003</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>0.53536099999999998</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>0.53622099999999995</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>0.53712099999999996</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>0.53758600000000001</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>0.53805999999999998</c:v>
-                </c:pt>
-                <c:pt idx="200">
-                  <c:v>0.53847500000000004</c:v>
-                </c:pt>
-                <c:pt idx="201">
-                  <c:v>0.53903999999999996</c:v>
-                </c:pt>
-                <c:pt idx="202">
-                  <c:v>0.54005999999999998</c:v>
-                </c:pt>
-                <c:pt idx="203">
-                  <c:v>0.54221900000000001</c:v>
-                </c:pt>
-                <c:pt idx="204">
                   <c:v>0.54278400000000004</c:v>
                 </c:pt>
               </c:numCache>
@@ -3063,607 +2907,430 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="232"/>
+                <c:pt idx="0">
+                  <c:v>269</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>268</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>267</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>266</c:v>
+                </c:pt>
                 <c:pt idx="4">
-                  <c:v>269</c:v>
+                  <c:v>265</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>268</c:v>
+                  <c:v>264</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>267</c:v>
+                  <c:v>262</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>266</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>265</c:v>
+                  <c:v>259</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>264</c:v>
+                  <c:v>258</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>257</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>246</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>244</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>242</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>241</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>239</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>238</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>237</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>231</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>204</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>204</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>231</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>238</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>239</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>242</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>259</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="88">
                   <c:v>262</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>260</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>259</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>258</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>257</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>252</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>254</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>253</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>250</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>251</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>248</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>246</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>245</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>244</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>243</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>242</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>241</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>239</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>238</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>237</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>236</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>235</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>234</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>233</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>232</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>231</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>229</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>228</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>227</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>226</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>225</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>224</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>223</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>222</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>221</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>223</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>219</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>218</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>222</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>219</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>218</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>217</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>216</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>215</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>214</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>213</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>212</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>211</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>209</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>208</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>207</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>206</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>205</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>204</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>203</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>202</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>201</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>199</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>198</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>197</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>196</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>195</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>194</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>193</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>192</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>197</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>198</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>201</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>202</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>203</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>204</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>205</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>206</c:v>
-                </c:pt>
                 <c:pt idx="89">
-                  <c:v>207</c:v>
+                  <c:v>271</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>208</c:v>
+                  <c:v>272</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>215</c:v>
+                  <c:v>273</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>209</c:v>
+                  <c:v>275</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>210</c:v>
+                  <c:v>276</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>211</c:v>
+                  <c:v>277</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>214</c:v>
+                  <c:v>279</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>216</c:v>
+                  <c:v>280</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>213</c:v>
+                  <c:v>281</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>217</c:v>
+                  <c:v>297</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>218</c:v>
+                  <c:v>298</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>219</c:v>
+                  <c:v>299</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>220</c:v>
+                  <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>221</c:v>
+                  <c:v>303</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>222</c:v>
+                  <c:v>304</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>223</c:v>
+                  <c:v>306</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>224</c:v>
+                  <c:v>317</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>225</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>226</c:v>
+                  <c:v>322</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>227</c:v>
+                  <c:v>323</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>228</c:v>
+                  <c:v>324</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>229</c:v>
+                  <c:v>327</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>230</c:v>
+                  <c:v>328</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>231</c:v>
+                  <c:v>342</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>233</c:v>
+                  <c:v>343</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>234</c:v>
+                  <c:v>344</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>236</c:v>
+                  <c:v>345</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>238</c:v>
+                  <c:v>349</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>239</c:v>
+                  <c:v>360</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>240</c:v>
+                  <c:v>361</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>242</c:v>
+                  <c:v>362</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>245</c:v>
+                  <c:v>364</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>251</c:v>
+                  <c:v>365</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>247</c:v>
+                  <c:v>366</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>249</c:v>
+                  <c:v>367</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>250</c:v>
+                  <c:v>369</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>248</c:v>
+                  <c:v>370</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>252</c:v>
+                  <c:v>372</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>253</c:v>
+                  <c:v>373</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>254</c:v>
+                  <c:v>374</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>255</c:v>
+                  <c:v>377</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>261</c:v>
+                  <c:v>379</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>256</c:v>
+                  <c:v>381</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>257</c:v>
+                  <c:v>382</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>258</c:v>
+                  <c:v>384</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>259</c:v>
+                  <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>260</c:v>
+                  <c:v>387</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>262</c:v>
+                  <c:v>388</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>271</c:v>
+                  <c:v>395</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>272</c:v>
+                  <c:v>390</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>273</c:v>
+                  <c:v>392</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>275</c:v>
+                  <c:v>396</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>276</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>277</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>279</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>278</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>280</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>281</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>297</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>298</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>299</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>302</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>303</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>304</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>306</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>308</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>309</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>310</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>316</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>312</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>315</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>317</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>320</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>322</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>323</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>324</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>327</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>328</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>342</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>343</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>344</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>345</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>340</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>346</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>347</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>348</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>349</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>352</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>351</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>357</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>359</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>360</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>361</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>362</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>364</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>365</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>366</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>367</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>369</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>370</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>372</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>373</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>374</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>377</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>379</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>381</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>382</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>384</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>386</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>387</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>388</c:v>
-                </c:pt>
-                <c:pt idx="200">
-                  <c:v>395</c:v>
-                </c:pt>
-                <c:pt idx="201">
-                  <c:v>390</c:v>
-                </c:pt>
-                <c:pt idx="202">
-                  <c:v>392</c:v>
-                </c:pt>
-                <c:pt idx="203">
-                  <c:v>396</c:v>
-                </c:pt>
-                <c:pt idx="204">
                   <c:v>397</c:v>
                 </c:pt>
               </c:numCache>
@@ -18404,16 +18071,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>156210</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>125730</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>52800</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>87090</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>37560</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>56610</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18854,7 +18521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36D6104B-C9E0-42E8-AA2A-689EB615114A}">
   <dimension ref="A1:AY73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR28" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="AR28" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="BL35" sqref="BL35"/>
     </sheetView>
   </sheetViews>
@@ -22835,7 +22502,7 @@
         <v>1.8107</v>
       </c>
       <c r="AX33">
-        <f t="shared" ref="AX33:AY96" si="29">AX32+0.1</f>
+        <f t="shared" ref="AX33:AY73" si="29">AX32+0.1</f>
         <v>0.2</v>
       </c>
       <c r="AY33">
@@ -29664,10 +29331,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{782205F6-3FFD-4338-A2A5-04E9D62A3720}">
-  <dimension ref="A1:E207"/>
+  <dimension ref="A1:G144"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+    <sheetView tabSelected="1" topLeftCell="D75" workbookViewId="0">
+      <selection activeCell="I78" sqref="I78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29701,6 +29368,12 @@
       <c r="B3">
         <v>269.64318511963302</v>
       </c>
+      <c r="D3">
+        <v>2.7025400000000002E-2</v>
+      </c>
+      <c r="E3">
+        <v>269</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -29709,6 +29382,12 @@
       <c r="B4">
         <v>262.00130236596402</v>
       </c>
+      <c r="D4">
+        <v>3.2099999999999997E-2</v>
+      </c>
+      <c r="E4">
+        <v>268</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -29717,6 +29396,12 @@
       <c r="B5">
         <v>256.53937987343602</v>
       </c>
+      <c r="D5">
+        <v>3.6417199999999997E-2</v>
+      </c>
+      <c r="E5">
+        <v>267</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -29725,6 +29410,12 @@
       <c r="B6">
         <v>252.17144479136999</v>
       </c>
+      <c r="D6">
+        <v>4.2013399999999999E-2</v>
+      </c>
+      <c r="E6">
+        <v>266</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -29734,10 +29425,10 @@
         <v>247.81152426908801</v>
       </c>
       <c r="D7">
-        <v>2.7025400000000002E-2</v>
+        <v>4.68511E-2</v>
       </c>
       <c r="E7">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -29748,10 +29439,10 @@
         <v>234.74378454191699</v>
       </c>
       <c r="D8">
-        <v>3.2099999999999997E-2</v>
+        <v>5.3877500000000002E-2</v>
       </c>
       <c r="E8">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -29762,10 +29453,10 @@
         <v>230.38386401963501</v>
       </c>
       <c r="D9">
-        <v>3.6417199999999997E-2</v>
+        <v>5.86314E-2</v>
       </c>
       <c r="E9">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -29776,10 +29467,10 @@
         <v>226.03195805713699</v>
       </c>
       <c r="D10">
-        <v>4.2013399999999999E-2</v>
+        <v>6.9841600000000004E-2</v>
       </c>
       <c r="E10">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -29790,10 +29481,10 @@
         <v>217.32814613214001</v>
       </c>
       <c r="D11">
-        <v>4.68511E-2</v>
+        <v>7.2817499999999993E-2</v>
       </c>
       <c r="E11">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -29804,10 +29495,10 @@
         <v>212.968225609857</v>
       </c>
       <c r="D12">
-        <v>5.3877500000000002E-2</v>
+        <v>7.8476400000000002E-2</v>
       </c>
       <c r="E12">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -29818,10 +29509,10 @@
         <v>206.44437394600101</v>
       </c>
       <c r="D13">
-        <v>5.86314E-2</v>
+        <v>8.2672899999999994E-2</v>
       </c>
       <c r="E13">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -29832,10 +29523,10 @@
         <v>196.64256733065</v>
       </c>
       <c r="D14">
-        <v>6.9841600000000004E-2</v>
+        <v>8.6788000000000004E-2</v>
       </c>
       <c r="E14">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -29846,10 +29537,10 @@
         <v>202.040373344909</v>
       </c>
       <c r="D15">
-        <v>7.2817499999999993E-2</v>
+        <v>0.123644</v>
       </c>
       <c r="E15">
-        <v>259</v>
+        <v>246</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -29860,10 +29551,10 @@
         <v>209.60611778063401</v>
       </c>
       <c r="D16">
-        <v>7.8476400000000002E-2</v>
+        <v>0.12687899999999999</v>
       </c>
       <c r="E16">
-        <v>258</v>
+        <v>245</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -29874,10 +29565,10 @@
         <v>215.04399659381201</v>
       </c>
       <c r="D17">
-        <v>8.2672899999999994E-2</v>
+        <v>0.13003600000000001</v>
       </c>
       <c r="E17">
-        <v>257</v>
+        <v>244</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -29888,10 +29579,10 @@
         <v>221.547811858209</v>
       </c>
       <c r="D18">
-        <v>8.6788000000000004E-2</v>
+        <v>0.13311300000000001</v>
       </c>
       <c r="E18">
-        <v>256</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -29902,10 +29593,10 @@
         <v>224.797715850461</v>
       </c>
       <c r="D19">
-        <v>9.3631400000000004E-2</v>
+        <v>0.13611100000000001</v>
       </c>
       <c r="E19">
-        <v>252</v>
+        <v>242</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -29916,10 +29607,10 @@
         <v>231.297523834966</v>
       </c>
       <c r="D20">
-        <v>9.4769500000000007E-2</v>
+        <v>0.13902900000000001</v>
       </c>
       <c r="E20">
-        <v>254</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -29930,10 +29621,10 @@
         <v>235.621378838222</v>
       </c>
       <c r="D21">
-        <v>9.8624500000000004E-2</v>
+        <v>0.14186799999999999</v>
       </c>
       <c r="E21">
-        <v>253</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -29944,10 +29635,10 @@
         <v>242.113172262944</v>
       </c>
       <c r="D22">
-        <v>0.10026</v>
+        <v>0.14462700000000001</v>
       </c>
       <c r="E22">
-        <v>250</v>
+        <v>239</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -29958,10 +29649,10 @@
         <v>246.441034546092</v>
       </c>
       <c r="D23">
-        <v>0.104265</v>
+        <v>0.14730599999999999</v>
       </c>
       <c r="E23">
-        <v>251</v>
+        <v>238</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -29972,10 +29663,10 @@
         <v>248.58092200831501</v>
       </c>
       <c r="D24">
-        <v>0.11694400000000001</v>
+        <v>0.14990500000000001</v>
       </c>
       <c r="E24">
-        <v>248</v>
+        <v>237</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -29986,10 +29677,10 @@
         <v>258.33063398507198</v>
       </c>
       <c r="D25">
-        <v>0.123644</v>
+        <v>0.152425</v>
       </c>
       <c r="E25">
-        <v>246</v>
+        <v>236</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -30000,10 +29691,10 @@
         <v>262.65849626822001</v>
       </c>
       <c r="D26">
-        <v>0.12687899999999999</v>
+        <v>0.154864</v>
       </c>
       <c r="E26">
-        <v>245</v>
+        <v>235</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -30014,10 +29705,10 @@
         <v>265.90038570068901</v>
       </c>
       <c r="D27">
-        <v>0.13003600000000001</v>
+        <v>0.157223</v>
       </c>
       <c r="E27">
-        <v>244</v>
+        <v>234</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -30028,10 +29719,10 @@
         <v>270.23626254362</v>
       </c>
       <c r="D28">
-        <v>0.13311300000000001</v>
+        <v>0.15950300000000001</v>
       </c>
       <c r="E28">
-        <v>243</v>
+        <v>233</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -30042,10 +29733,10 @@
         <v>272.39618640530199</v>
       </c>
       <c r="D29">
-        <v>0.13611100000000001</v>
+        <v>0.16170300000000001</v>
       </c>
       <c r="E29">
-        <v>242</v>
+        <v>232</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -30056,10 +29747,10 @@
         <v>275.64609039755499</v>
       </c>
       <c r="D30">
-        <v>0.13902900000000001</v>
+        <v>0.163822</v>
       </c>
       <c r="E30">
-        <v>241</v>
+        <v>231</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -30070,10 +29761,10 @@
         <v>277.80601425923697</v>
       </c>
       <c r="D31">
-        <v>0.14186799999999999</v>
+        <v>0.16586200000000001</v>
       </c>
       <c r="E31">
-        <v>240</v>
+        <v>230</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -30084,10 +29775,10 @@
         <v>279.95391628124401</v>
       </c>
       <c r="D32">
-        <v>0.14462700000000001</v>
+        <v>0.167822</v>
       </c>
       <c r="E32">
-        <v>239</v>
+        <v>229</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -30098,10 +29789,10 @@
         <v>288.61765540732301</v>
       </c>
       <c r="D33">
-        <v>0.14730599999999999</v>
+        <v>0.16970099999999999</v>
       </c>
       <c r="E33">
-        <v>238</v>
+        <v>228</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -30112,10 +29803,10 @@
         <v>292.94151041057899</v>
       </c>
       <c r="D34">
-        <v>0.14990500000000001</v>
+        <v>0.17150099999999999</v>
       </c>
       <c r="E34">
-        <v>237</v>
+        <v>227</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -30126,10 +29817,10 @@
         <v>292.91746673122799</v>
       </c>
       <c r="D35">
-        <v>0.152425</v>
+        <v>0.17322100000000001</v>
       </c>
       <c r="E35">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -30140,10 +29831,10 @@
         <v>300.50324756641203</v>
       </c>
       <c r="D36">
-        <v>0.154864</v>
+        <v>0.17486099999999999</v>
       </c>
       <c r="E36">
-        <v>235</v>
+        <v>225</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -30154,10 +29845,10 @@
         <v>304.83511712945102</v>
       </c>
       <c r="D37">
-        <v>0.157223</v>
+        <v>0.19392699999999999</v>
       </c>
       <c r="E37">
-        <v>234</v>
+        <v>216</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -30168,10 +29859,10 @@
         <v>310.24494498338601</v>
       </c>
       <c r="D38">
-        <v>0.15950300000000001</v>
+        <v>0.19553400000000001</v>
       </c>
       <c r="E38">
-        <v>233</v>
+        <v>215</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -30182,10 +29873,10 @@
         <v>316.73273112821602</v>
       </c>
       <c r="D39">
-        <v>0.16170300000000001</v>
+        <v>0.19714699999999999</v>
       </c>
       <c r="E39">
-        <v>232</v>
+        <v>214</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -30196,10 +29887,10 @@
         <v>323.224524552937</v>
       </c>
       <c r="D40">
-        <v>0.163822</v>
+        <v>0.198765</v>
       </c>
       <c r="E40">
-        <v>231</v>
+        <v>213</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -30210,10 +29901,10 @@
         <v>330.81431266801297</v>
       </c>
       <c r="D41">
-        <v>0.16586200000000001</v>
+        <v>0.20039000000000001</v>
       </c>
       <c r="E41">
-        <v>230</v>
+        <v>212</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -30224,10 +29915,10 @@
         <v>337.30610609273498</v>
       </c>
       <c r="D42">
-        <v>0.167822</v>
+        <v>0.20202100000000001</v>
       </c>
       <c r="E42">
-        <v>229</v>
+        <v>211</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -30238,10 +29929,10 @@
         <v>342.70791938688598</v>
       </c>
       <c r="D43">
-        <v>0.16970099999999999</v>
+        <v>0.20530100000000001</v>
       </c>
       <c r="E43">
-        <v>228</v>
+        <v>209</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -30252,10 +29943,10 @@
         <v>345.93377969978701</v>
       </c>
       <c r="D44">
-        <v>0.17150099999999999</v>
+        <v>0.20695</v>
       </c>
       <c r="E44">
-        <v>227</v>
+        <v>208</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -30266,10 +29957,10 @@
         <v>351.33158571404698</v>
       </c>
       <c r="D45">
-        <v>0.17322100000000001</v>
+        <v>0.20860500000000001</v>
       </c>
       <c r="E45">
-        <v>226</v>
+        <v>207</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -30280,10 +29971,10 @@
         <v>354.55744602694801</v>
       </c>
       <c r="D46">
-        <v>0.17486099999999999</v>
+        <v>0.21026600000000001</v>
       </c>
       <c r="E46">
-        <v>225</v>
+        <v>206</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -30294,10 +29985,10 @@
         <v>362.10716134310599</v>
       </c>
       <c r="D47">
-        <v>0.17642099999999999</v>
+        <v>0.21193300000000001</v>
       </c>
       <c r="E47">
-        <v>224</v>
+        <v>205</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -30308,10 +29999,10 @@
         <v>365.35305805546699</v>
       </c>
       <c r="D48">
-        <v>0.1779</v>
+        <v>0.21360599999999999</v>
       </c>
       <c r="E48">
-        <v>223</v>
+        <v>204</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -30322,10 +30013,10 @@
         <v>365.325007096224</v>
       </c>
       <c r="D49">
-        <v>0.17929999999999999</v>
+        <v>0.215285</v>
       </c>
       <c r="E49">
-        <v>222</v>
+        <v>203</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -30336,10 +30027,10 @@
         <v>366.354878028418</v>
       </c>
       <c r="D50">
-        <v>0.18062</v>
+        <v>0.216969</v>
       </c>
       <c r="E50">
-        <v>221</v>
+        <v>202</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -30350,10 +30041,10 @@
         <v>371.82882236062102</v>
       </c>
       <c r="D51">
-        <v>0.18185999999999999</v>
+        <v>0.21865999999999999</v>
       </c>
       <c r="E51">
-        <v>220</v>
+        <v>201</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -30364,10 +30055,10 @@
         <v>379.42662503548098</v>
       </c>
       <c r="D52">
-        <v>0.18284700000000001</v>
+        <v>0.220357</v>
       </c>
       <c r="E52">
-        <v>223</v>
+        <v>200</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -30378,10 +30069,10 @@
         <v>388.102386001235</v>
       </c>
       <c r="D53">
-        <v>0.18301999999999999</v>
+        <v>0.22206000000000001</v>
       </c>
       <c r="E53">
-        <v>219</v>
+        <v>199</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -30392,10 +30083,10 @@
         <v>392.43024828438303</v>
       </c>
       <c r="D54">
-        <v>0.18410000000000001</v>
+        <v>0.223769</v>
       </c>
       <c r="E54">
-        <v>218</v>
+        <v>198</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -30406,1225 +30097,724 @@
         <v>396.77013240720601</v>
       </c>
       <c r="D55">
-        <v>0.18441199999999999</v>
+        <v>0.22548399999999999</v>
       </c>
       <c r="E55">
-        <v>222</v>
+        <v>197</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D56">
-        <v>0.189142</v>
+        <v>0.22720499999999999</v>
       </c>
       <c r="E56">
-        <v>219</v>
+        <v>196</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D57">
-        <v>0.19073100000000001</v>
+        <v>0.228932</v>
       </c>
       <c r="E57">
-        <v>218</v>
+        <v>195</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D58">
-        <v>0.192326</v>
+        <v>0.23066500000000001</v>
       </c>
       <c r="E58">
-        <v>217</v>
+        <v>194</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D59">
-        <v>0.19392699999999999</v>
+        <v>0.232404</v>
       </c>
       <c r="E59">
-        <v>216</v>
+        <v>193</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D60">
-        <v>0.19553400000000001</v>
+        <v>0.234149</v>
       </c>
       <c r="E60">
-        <v>215</v>
+        <v>192</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D61">
-        <v>0.19714699999999999</v>
+        <v>0.24410200000000001</v>
       </c>
       <c r="E61">
-        <v>214</v>
+        <v>197</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D62">
-        <v>0.198765</v>
+        <v>0.24571200000000001</v>
       </c>
       <c r="E62">
-        <v>213</v>
+        <v>198</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D63">
-        <v>0.20039000000000001</v>
+        <v>0.24895600000000001</v>
       </c>
       <c r="E63">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D64">
-        <v>0.20202100000000001</v>
+        <v>0.25058999999999998</v>
       </c>
       <c r="E64">
-        <v>211</v>
+        <v>201</v>
       </c>
     </row>
     <row r="65" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D65">
-        <v>0.20530100000000001</v>
+        <v>0.25223200000000001</v>
       </c>
       <c r="E65">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="66" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D66">
-        <v>0.20695</v>
+        <v>0.253882</v>
       </c>
       <c r="E66">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="67" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D67">
-        <v>0.20860500000000001</v>
+        <v>0.25553999999999999</v>
       </c>
       <c r="E67">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="68" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D68">
-        <v>0.21026600000000001</v>
+        <v>0.25827800000000001</v>
       </c>
       <c r="E68">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="69" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D69">
-        <v>0.21193300000000001</v>
+        <v>0.25888</v>
       </c>
       <c r="E69">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="70" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D70">
-        <v>0.21360599999999999</v>
+        <v>0.27629599999999999</v>
       </c>
       <c r="E70">
-        <v>204</v>
+        <v>213</v>
       </c>
     </row>
     <row r="71" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D71">
-        <v>0.215285</v>
+        <v>0.28675099999999998</v>
       </c>
       <c r="E71">
-        <v>203</v>
+        <v>222</v>
       </c>
     </row>
     <row r="72" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D72">
-        <v>0.216969</v>
+        <v>0.28856100000000001</v>
       </c>
       <c r="E72">
-        <v>202</v>
+        <v>223</v>
       </c>
     </row>
     <row r="73" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D73">
-        <v>0.21865999999999999</v>
+        <v>0.290379</v>
       </c>
       <c r="E73">
-        <v>201</v>
+        <v>224</v>
       </c>
     </row>
     <row r="74" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D74">
-        <v>0.220357</v>
+        <v>0.29220499999999999</v>
       </c>
       <c r="E74">
-        <v>200</v>
+        <v>225</v>
       </c>
     </row>
     <row r="75" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D75">
-        <v>0.22206000000000001</v>
+        <v>0.29403800000000002</v>
       </c>
       <c r="E75">
-        <v>199</v>
+        <v>226</v>
       </c>
     </row>
     <row r="76" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D76">
-        <v>0.223769</v>
+        <v>0.29587999999999998</v>
       </c>
       <c r="E76">
-        <v>198</v>
+        <v>227</v>
       </c>
     </row>
     <row r="77" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D77">
-        <v>0.22548399999999999</v>
+        <v>0.29772999999999999</v>
       </c>
       <c r="E77">
-        <v>197</v>
+        <v>228</v>
       </c>
     </row>
     <row r="78" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D78">
-        <v>0.22720499999999999</v>
+        <v>0.29958800000000002</v>
       </c>
       <c r="E78">
-        <v>196</v>
+        <v>229</v>
       </c>
     </row>
     <row r="79" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D79">
-        <v>0.228932</v>
+        <v>0.301454</v>
       </c>
       <c r="E79">
-        <v>195</v>
+        <v>230</v>
       </c>
     </row>
     <row r="80" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D80">
-        <v>0.23066500000000001</v>
+        <v>0.30332799999999999</v>
       </c>
       <c r="E80">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="81" spans="4:5" x14ac:dyDescent="0.3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="81" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D81">
-        <v>0.232404</v>
+        <v>0.30709999999999998</v>
       </c>
       <c r="E81">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="82" spans="4:5" x14ac:dyDescent="0.3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="82" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D82">
-        <v>0.234149</v>
+        <v>0.30899799999999999</v>
       </c>
       <c r="E82">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="83" spans="4:5" x14ac:dyDescent="0.3">
+        <v>234</v>
+      </c>
+      <c r="G82" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="83" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D83">
-        <v>0.24410200000000001</v>
+        <v>0.31281799999999998</v>
       </c>
       <c r="E83">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="84" spans="4:5" x14ac:dyDescent="0.3">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="84" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D84">
-        <v>0.24571200000000001</v>
+        <v>0.31667000000000001</v>
       </c>
       <c r="E84">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="85" spans="4:5" x14ac:dyDescent="0.3">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="85" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D85">
-        <v>0.24895600000000001</v>
+        <v>0.318608</v>
       </c>
       <c r="E85">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="86" spans="4:5" x14ac:dyDescent="0.3">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="86" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D86">
-        <v>0.25058999999999998</v>
+        <v>0.32055400000000001</v>
       </c>
       <c r="E86">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="87" spans="4:5" x14ac:dyDescent="0.3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="87" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D87">
-        <v>0.25223200000000001</v>
+        <v>0.32446999999999998</v>
       </c>
       <c r="E87">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="88" spans="4:5" x14ac:dyDescent="0.3">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="88" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D88">
-        <v>0.253882</v>
+        <v>0.330403</v>
       </c>
       <c r="E88">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="89" spans="4:5" x14ac:dyDescent="0.3">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="89" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D89">
-        <v>0.25553999999999999</v>
+        <v>0.35904599999999998</v>
       </c>
       <c r="E89">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="90" spans="4:5" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="90" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D90">
-        <v>0.25827800000000001</v>
+        <v>0.36115199999999997</v>
       </c>
       <c r="E90">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="91" spans="4:5" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="91" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D91">
-        <v>0.25888</v>
+        <v>0.36538799999999999</v>
       </c>
       <c r="E91">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="92" spans="4:5" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="92" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D92">
-        <v>0.26056200000000002</v>
+        <v>0.38484600000000002</v>
       </c>
       <c r="E92">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="93" spans="4:5" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="93" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D93">
-        <v>0.26225199999999999</v>
+        <v>0.387048</v>
       </c>
       <c r="E93">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="94" spans="4:5" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="94" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D94">
-        <v>0.26235700000000001</v>
+        <v>0.38925799999999999</v>
       </c>
       <c r="E94">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="95" spans="4:5" x14ac:dyDescent="0.3">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="95" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D95">
-        <v>0.26394899999999999</v>
+        <v>0.39370100000000002</v>
       </c>
       <c r="E95">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="96" spans="4:5" x14ac:dyDescent="0.3">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="96" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D96">
-        <v>0.26565499999999997</v>
+        <v>0.39593499999999998</v>
       </c>
       <c r="E96">
-        <v>210</v>
+        <v>276</v>
       </c>
     </row>
     <row r="97" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D97">
-        <v>0.26736900000000002</v>
+        <v>0.398177</v>
       </c>
       <c r="E97">
-        <v>211</v>
+        <v>277</v>
       </c>
     </row>
     <row r="98" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D98">
-        <v>0.272559</v>
+        <v>0.40268500000000002</v>
       </c>
       <c r="E98">
-        <v>214</v>
+        <v>279</v>
       </c>
     </row>
     <row r="99" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D99">
-        <v>0.276059</v>
+        <v>0.40495100000000001</v>
       </c>
       <c r="E99">
-        <v>216</v>
+        <v>280</v>
       </c>
     </row>
     <row r="100" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D100">
-        <v>0.27629599999999999</v>
+        <v>0.407225</v>
       </c>
       <c r="E100">
-        <v>213</v>
+        <v>281</v>
       </c>
     </row>
     <row r="101" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D101">
-        <v>0.27782099999999998</v>
+        <v>0.42696200000000001</v>
       </c>
       <c r="E101">
-        <v>217</v>
+        <v>297</v>
       </c>
     </row>
     <row r="102" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D102">
-        <v>0.27959099999999998</v>
+        <v>0.42812600000000001</v>
       </c>
       <c r="E102">
-        <v>218</v>
+        <v>298</v>
       </c>
     </row>
     <row r="103" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D103">
-        <v>0.28136899999999998</v>
+        <v>0.42928899999999998</v>
       </c>
       <c r="E103">
-        <v>219</v>
+        <v>299</v>
       </c>
     </row>
     <row r="104" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D104">
-        <v>0.28315499999999999</v>
+        <v>0.43276599999999998</v>
       </c>
       <c r="E104">
-        <v>220</v>
+        <v>302</v>
       </c>
     </row>
     <row r="105" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D105">
-        <v>0.28494900000000001</v>
+        <v>0.43392199999999997</v>
       </c>
       <c r="E105">
-        <v>221</v>
+        <v>303</v>
       </c>
     </row>
     <row r="106" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D106">
-        <v>0.28675099999999998</v>
+        <v>0.43507499999999999</v>
       </c>
       <c r="E106">
-        <v>222</v>
+        <v>304</v>
       </c>
     </row>
     <row r="107" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D107">
-        <v>0.28856100000000001</v>
+        <v>0.43737700000000002</v>
       </c>
       <c r="E107">
-        <v>223</v>
+        <v>306</v>
       </c>
     </row>
     <row r="108" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D108">
-        <v>0.290379</v>
+        <v>0.449909</v>
       </c>
       <c r="E108">
-        <v>224</v>
+        <v>317</v>
       </c>
     </row>
     <row r="109" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D109">
-        <v>0.29220499999999999</v>
+        <v>0.453289</v>
       </c>
       <c r="E109">
-        <v>225</v>
+        <v>320</v>
       </c>
     </row>
     <row r="110" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D110">
-        <v>0.29403800000000002</v>
+        <v>0.45553500000000002</v>
       </c>
       <c r="E110">
-        <v>226</v>
+        <v>322</v>
       </c>
     </row>
     <row r="111" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D111">
-        <v>0.29587999999999998</v>
+        <v>0.45665299999999998</v>
       </c>
       <c r="E111">
-        <v>227</v>
+        <v>323</v>
       </c>
     </row>
     <row r="112" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D112">
-        <v>0.29772999999999999</v>
+        <v>0.45777000000000001</v>
       </c>
       <c r="E112">
-        <v>228</v>
+        <v>324</v>
       </c>
     </row>
     <row r="113" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D113">
-        <v>0.29958800000000002</v>
+        <v>0.46111200000000002</v>
       </c>
       <c r="E113">
-        <v>229</v>
+        <v>327</v>
       </c>
     </row>
     <row r="114" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D114">
-        <v>0.301454</v>
+        <v>0.46222299999999999</v>
       </c>
       <c r="E114">
-        <v>230</v>
+        <v>328</v>
       </c>
     </row>
     <row r="115" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D115">
-        <v>0.30332799999999999</v>
+        <v>0.47289599999999998</v>
       </c>
       <c r="E115">
-        <v>231</v>
+        <v>342</v>
       </c>
     </row>
     <row r="116" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D116">
-        <v>0.30709999999999998</v>
+        <v>0.47489100000000001</v>
       </c>
       <c r="E116">
-        <v>233</v>
+        <v>343</v>
       </c>
     </row>
     <row r="117" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D117">
-        <v>0.30899799999999999</v>
+        <v>0.47689999999999999</v>
       </c>
       <c r="E117">
-        <v>234</v>
+        <v>344</v>
       </c>
     </row>
     <row r="118" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D118">
-        <v>0.31281799999999998</v>
+        <v>0.47892299999999999</v>
       </c>
       <c r="E118">
-        <v>236</v>
+        <v>345</v>
       </c>
     </row>
     <row r="119" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D119">
-        <v>0.31667000000000001</v>
+        <v>0.48715399999999998</v>
       </c>
       <c r="E119">
-        <v>238</v>
+        <v>349</v>
       </c>
     </row>
     <row r="120" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D120">
-        <v>0.318608</v>
+        <v>0.51049100000000003</v>
       </c>
       <c r="E120">
-        <v>239</v>
+        <v>360</v>
       </c>
     </row>
     <row r="121" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D121">
-        <v>0.32055400000000001</v>
+        <v>0.51319199999999998</v>
       </c>
       <c r="E121">
-        <v>240</v>
+        <v>361</v>
       </c>
     </row>
     <row r="122" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D122">
-        <v>0.32446999999999998</v>
+        <v>0.51545300000000005</v>
       </c>
       <c r="E122">
-        <v>242</v>
+        <v>362</v>
       </c>
     </row>
     <row r="123" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D123">
-        <v>0.330403</v>
+        <v>0.52001600000000003</v>
       </c>
       <c r="E123">
-        <v>245</v>
+        <v>364</v>
       </c>
     </row>
     <row r="124" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D124">
-        <v>0.33417400000000003</v>
+        <v>0.52231899999999998</v>
       </c>
       <c r="E124">
-        <v>251</v>
+        <v>365</v>
       </c>
     </row>
     <row r="125" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D125">
-        <v>0.334399</v>
+        <v>0.52851999999999999</v>
       </c>
       <c r="E125">
-        <v>247</v>
+        <v>366</v>
       </c>
     </row>
     <row r="126" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D126">
-        <v>0.33842699999999998</v>
+        <v>0.53018699999999996</v>
       </c>
       <c r="E126">
-        <v>249</v>
+        <v>367</v>
       </c>
     </row>
     <row r="127" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D127">
-        <v>0.34045300000000001</v>
+        <v>0.53074699999999997</v>
       </c>
       <c r="E127">
-        <v>250</v>
+        <v>369</v>
       </c>
     </row>
     <row r="128" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D128">
-        <v>0.34338400000000002</v>
+        <v>0.53104200000000001</v>
       </c>
       <c r="E128">
-        <v>248</v>
+        <v>370</v>
       </c>
     </row>
     <row r="129" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D129">
-        <v>0.34369699999999997</v>
+        <v>0.53166199999999997</v>
       </c>
       <c r="E129">
-        <v>252</v>
+        <v>372</v>
       </c>
     </row>
     <row r="130" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D130">
-        <v>0.34657900000000003</v>
+        <v>0.53198699999999999</v>
       </c>
       <c r="E130">
-        <v>253</v>
+        <v>373</v>
       </c>
     </row>
     <row r="131" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D131">
-        <v>0.34863699999999997</v>
+        <v>0.53232199999999996</v>
       </c>
       <c r="E131">
-        <v>254</v>
+        <v>374</v>
       </c>
     </row>
     <row r="132" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D132">
-        <v>0.35070299999999999</v>
+        <v>0.53338600000000003</v>
       </c>
       <c r="E132">
-        <v>255</v>
+        <v>377</v>
       </c>
     </row>
     <row r="133" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D133">
-        <v>0.35108099999999998</v>
+        <v>0.53414600000000001</v>
       </c>
       <c r="E133">
-        <v>261</v>
+        <v>379</v>
       </c>
     </row>
     <row r="134" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D134">
-        <v>0.35277700000000001</v>
+        <v>0.53494600000000003</v>
       </c>
       <c r="E134">
-        <v>256</v>
+        <v>381</v>
       </c>
     </row>
     <row r="135" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D135">
-        <v>0.35485899999999998</v>
+        <v>0.53536099999999998</v>
       </c>
       <c r="E135">
-        <v>257</v>
+        <v>382</v>
       </c>
     </row>
     <row r="136" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D136">
-        <v>0.35694900000000002</v>
+        <v>0.53622099999999995</v>
       </c>
       <c r="E136">
-        <v>258</v>
+        <v>384</v>
       </c>
     </row>
     <row r="137" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D137">
-        <v>0.35904599999999998</v>
+        <v>0.53712099999999996</v>
       </c>
       <c r="E137">
-        <v>259</v>
+        <v>386</v>
       </c>
     </row>
     <row r="138" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D138">
-        <v>0.36115199999999997</v>
+        <v>0.53758600000000001</v>
       </c>
       <c r="E138">
-        <v>260</v>
+        <v>387</v>
       </c>
     </row>
     <row r="139" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D139">
-        <v>0.36538799999999999</v>
+        <v>0.53805999999999998</v>
       </c>
       <c r="E139">
-        <v>262</v>
+        <v>388</v>
       </c>
     </row>
     <row r="140" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D140">
-        <v>0.38484600000000002</v>
+        <v>0.53847500000000004</v>
       </c>
       <c r="E140">
-        <v>271</v>
+        <v>395</v>
       </c>
     </row>
     <row r="141" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D141">
-        <v>0.387048</v>
+        <v>0.53903999999999996</v>
       </c>
       <c r="E141">
-        <v>272</v>
+        <v>390</v>
       </c>
     </row>
     <row r="142" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D142">
-        <v>0.38925799999999999</v>
+        <v>0.54005999999999998</v>
       </c>
       <c r="E142">
-        <v>273</v>
+        <v>392</v>
       </c>
     </row>
     <row r="143" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D143">
-        <v>0.39370100000000002</v>
+        <v>0.54221900000000001</v>
       </c>
       <c r="E143">
-        <v>275</v>
+        <v>396</v>
       </c>
     </row>
     <row r="144" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D144">
-        <v>0.39593499999999998</v>
+        <v>0.54278400000000004</v>
       </c>
       <c r="E144">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="145" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D145">
-        <v>0.398177</v>
-      </c>
-      <c r="E145">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="146" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D146">
-        <v>0.40268500000000002</v>
-      </c>
-      <c r="E146">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="147" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D147">
-        <v>0.40348800000000001</v>
-      </c>
-      <c r="E147">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="148" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D148">
-        <v>0.40495100000000001</v>
-      </c>
-      <c r="E148">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="149" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D149">
-        <v>0.407225</v>
-      </c>
-      <c r="E149">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="150" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D150">
-        <v>0.42696200000000001</v>
-      </c>
-      <c r="E150">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="151" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D151">
-        <v>0.42812600000000001</v>
-      </c>
-      <c r="E151">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="152" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D152">
-        <v>0.42928899999999998</v>
-      </c>
-      <c r="E152">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="153" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D153">
-        <v>0.43276599999999998</v>
-      </c>
-      <c r="E153">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="154" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D154">
-        <v>0.43392199999999997</v>
-      </c>
-      <c r="E154">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="155" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D155">
-        <v>0.43507499999999999</v>
-      </c>
-      <c r="E155">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="156" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D156">
-        <v>0.43737700000000002</v>
-      </c>
-      <c r="E156">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="157" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D157">
-        <v>0.43967200000000001</v>
-      </c>
-      <c r="E157">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="158" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D158">
-        <v>0.44081700000000001</v>
-      </c>
-      <c r="E158">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="159" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D159">
-        <v>0.44195899999999999</v>
-      </c>
-      <c r="E159">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="160" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D160">
-        <v>0.44416699999999998</v>
-      </c>
-      <c r="E160">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="161" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D161">
-        <v>0.44424000000000002</v>
-      </c>
-      <c r="E161">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="162" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D162">
-        <v>0.44764700000000002</v>
-      </c>
-      <c r="E162">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="163" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D163">
-        <v>0.449909</v>
-      </c>
-      <c r="E163">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="164" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D164">
-        <v>0.453289</v>
-      </c>
-      <c r="E164">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="165" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D165">
-        <v>0.45553500000000002</v>
-      </c>
-      <c r="E165">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="166" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D166">
-        <v>0.45665299999999998</v>
-      </c>
-      <c r="E166">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="167" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D167">
-        <v>0.45777000000000001</v>
-      </c>
-      <c r="E167">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="168" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D168">
-        <v>0.46111200000000002</v>
-      </c>
-      <c r="E168">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="169" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D169">
-        <v>0.46222299999999999</v>
-      </c>
-      <c r="E169">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="170" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D170">
-        <v>0.47289599999999998</v>
-      </c>
-      <c r="E170">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="171" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D171">
-        <v>0.47489100000000001</v>
-      </c>
-      <c r="E171">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="172" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D172">
-        <v>0.47689999999999999</v>
-      </c>
-      <c r="E172">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="173" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D173">
-        <v>0.47892299999999999</v>
-      </c>
-      <c r="E173">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="174" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D174">
-        <v>0.48065600000000003</v>
-      </c>
-      <c r="E174">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="175" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D175">
-        <v>0.48096</v>
-      </c>
-      <c r="E175">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="176" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D176">
-        <v>0.48301100000000002</v>
-      </c>
-      <c r="E176">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="177" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D177">
-        <v>0.48507499999999998</v>
-      </c>
-      <c r="E177">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="178" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D178">
-        <v>0.48715399999999998</v>
-      </c>
-      <c r="E178">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="179" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D179">
-        <v>0.493475</v>
-      </c>
-      <c r="E179">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="180" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D180">
-        <v>0.500143</v>
-      </c>
-      <c r="E180">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="181" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D181">
-        <v>0.50428899999999999</v>
-      </c>
-      <c r="E181">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="182" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D182">
-        <v>0.50871299999999997</v>
-      </c>
-      <c r="E182">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="183" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D183">
-        <v>0.51049100000000003</v>
-      </c>
-      <c r="E183">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="184" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D184">
-        <v>0.51319199999999998</v>
-      </c>
-      <c r="E184">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="185" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D185">
-        <v>0.51545300000000005</v>
-      </c>
-      <c r="E185">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="186" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D186">
-        <v>0.52001600000000003</v>
-      </c>
-      <c r="E186">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="187" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D187">
-        <v>0.52231899999999998</v>
-      </c>
-      <c r="E187">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="188" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D188">
-        <v>0.52851999999999999</v>
-      </c>
-      <c r="E188">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="189" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D189">
-        <v>0.53018699999999996</v>
-      </c>
-      <c r="E189">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="190" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D190">
-        <v>0.53074699999999997</v>
-      </c>
-      <c r="E190">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="191" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D191">
-        <v>0.53104200000000001</v>
-      </c>
-      <c r="E191">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="192" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D192">
-        <v>0.53166199999999997</v>
-      </c>
-      <c r="E192">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="193" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D193">
-        <v>0.53198699999999999</v>
-      </c>
-      <c r="E193">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="194" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D194">
-        <v>0.53232199999999996</v>
-      </c>
-      <c r="E194">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="195" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D195">
-        <v>0.53338600000000003</v>
-      </c>
-      <c r="E195">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="196" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D196">
-        <v>0.53414600000000001</v>
-      </c>
-      <c r="E196">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="197" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D197">
-        <v>0.53494600000000003</v>
-      </c>
-      <c r="E197">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="198" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D198">
-        <v>0.53536099999999998</v>
-      </c>
-      <c r="E198">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="199" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D199">
-        <v>0.53622099999999995</v>
-      </c>
-      <c r="E199">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="200" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D200">
-        <v>0.53712099999999996</v>
-      </c>
-      <c r="E200">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="201" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D201">
-        <v>0.53758600000000001</v>
-      </c>
-      <c r="E201">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="202" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D202">
-        <v>0.53805999999999998</v>
-      </c>
-      <c r="E202">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="203" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D203">
-        <v>0.53847500000000004</v>
-      </c>
-      <c r="E203">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="204" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D204">
-        <v>0.53903999999999996</v>
-      </c>
-      <c r="E204">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="205" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D205">
-        <v>0.54005999999999998</v>
-      </c>
-      <c r="E205">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="206" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D206">
-        <v>0.54221900000000001</v>
-      </c>
-      <c r="E206">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="207" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D207">
-        <v>0.54278400000000004</v>
-      </c>
-      <c r="E207">
         <v>397</v>
       </c>
     </row>
@@ -31647,6 +30837,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="49fa8af8-517d-491f-a3d5-7cf68fb985f9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010054E8EBE579ED724DA6862405C7970F81" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="86c5e3b6225d101e522740491cefce85">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="49fa8af8-517d-491f-a3d5-7cf68fb985f9" xmlns:ns4="5d848a0f-dbe6-471c-a407-bb7a402dc859" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a6c024ab2e87b0647c7181ba4225cb0c" ns3:_="" ns4:_="">
     <xsd:import namespace="49fa8af8-517d-491f-a3d5-7cf68fb985f9"/>
@@ -31875,14 +31073,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="49fa8af8-517d-491f-a3d5-7cf68fb985f9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C69340E-2751-479C-A826-08E03A5B21D5}">
   <ds:schemaRefs>
@@ -31892,6 +31082,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AC3A44B-2E43-454A-BBA7-EBDF5C93942F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5d848a0f-dbe6-471c-a407-bb7a402dc859"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="49fa8af8-517d-491f-a3d5-7cf68fb985f9"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE99C8A8-65B8-4C1C-AC8C-1B7793729012}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -31908,21 +31115,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AC3A44B-2E43-454A-BBA7-EBDF5C93942F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5d848a0f-dbe6-471c-a407-bb7a402dc859"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="49fa8af8-517d-491f-a3d5-7cf68fb985f9"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
changes made in final paper
</commit_message>
<xml_diff>
--- a/CURRENT WORK/SALT WORK - CODES/N = 3/LiCl - Done/Test Excelsheet for LiCl n=3.xlsx
+++ b/CURRENT WORK/SALT WORK - CODES/N = 3/LiCl - Done/Test Excelsheet for LiCl n=3.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{93867D99-CC85-4827-9ADE-CAAC7A14BBDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68E072C8-71B5-4E74-8C9C-461709A2BE29}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{E88A55E1-2FE1-4A75-8B73-96F5B642C0CF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{E88A55E1-2FE1-4A75-8B73-96F5B642C0CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet for finding Unknown LiCl" sheetId="1" r:id="rId1"/>
@@ -18043,6 +18043,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
 <rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
   <global>
@@ -18456,7 +18460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36D6104B-C9E0-42E8-AA2A-689EB615114A}">
   <dimension ref="A1:AY73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR37" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="AR37" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="BL35" sqref="BL35"/>
     </sheetView>
   </sheetViews>
@@ -27070,7 +27074,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2AA8488-41ED-4A9D-8056-1830263C77F2}">
   <dimension ref="A1:W89"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="116" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="V6" sqref="V6:W37"/>
     </sheetView>
   </sheetViews>
@@ -30772,6 +30776,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="49fa8af8-517d-491f-a3d5-7cf68fb985f9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010054E8EBE579ED724DA6862405C7970F81" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="86c5e3b6225d101e522740491cefce85">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="49fa8af8-517d-491f-a3d5-7cf68fb985f9" xmlns:ns4="5d848a0f-dbe6-471c-a407-bb7a402dc859" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a6c024ab2e87b0647c7181ba4225cb0c" ns3:_="" ns4:_="">
     <xsd:import namespace="49fa8af8-517d-491f-a3d5-7cf68fb985f9"/>
@@ -31000,14 +31012,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="49fa8af8-517d-491f-a3d5-7cf68fb985f9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C69340E-2751-479C-A826-08E03A5B21D5}">
   <ds:schemaRefs>
@@ -31017,6 +31021,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AC3A44B-2E43-454A-BBA7-EBDF5C93942F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5d848a0f-dbe6-471c-a407-bb7a402dc859"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="49fa8af8-517d-491f-a3d5-7cf68fb985f9"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE99C8A8-65B8-4C1C-AC8C-1B7793729012}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -31033,21 +31054,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AC3A44B-2E43-454A-BBA7-EBDF5C93942F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5d848a0f-dbe6-471c-a407-bb7a402dc859"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="49fa8af8-517d-491f-a3d5-7cf68fb985f9"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[add]: folder and files added for N=2
</commit_message>
<xml_diff>
--- a/CURRENT WORK/SALT WORK - CODES/N = 3/LiCl - Done/Test Excelsheet for LiCl n=3.xlsx
+++ b/CURRENT WORK/SALT WORK - CODES/N = 3/LiCl - Done/Test Excelsheet for LiCl n=3.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{93867D99-CC85-4827-9ADE-CAAC7A14BBDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68E072C8-71B5-4E74-8C9C-461709A2BE29}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="708" activeTab="1" xr2:uid="{E88A55E1-2FE1-4A75-8B73-96F5B642C0CF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="708" xr2:uid="{E88A55E1-2FE1-4A75-8B73-96F5B642C0CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet for finding Unknown LiCl" sheetId="1" r:id="rId1"/>
@@ -18460,8 +18460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36D6104B-C9E0-42E8-AA2A-689EB615114A}">
   <dimension ref="A1:AY73"/>
   <sheetViews>
-    <sheetView topLeftCell="AR2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BL35" sqref="BL35"/>
+    <sheetView tabSelected="1" topLeftCell="AP40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AU32" sqref="AU32:AV59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -26634,7 +26634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{780679C4-5DB7-4A9B-9A75-6C5862E42C04}">
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
@@ -30996,20 +30996,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="49fa8af8-517d-491f-a3d5-7cf68fb985f9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="49fa8af8-517d-491f-a3d5-7cf68fb985f9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -31032,6 +31032,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C69340E-2751-479C-A826-08E03A5B21D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AC3A44B-2E43-454A-BBA7-EBDF5C93942F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -31046,12 +31054,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C69340E-2751-479C-A826-08E03A5B21D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>